<commit_message>
subscription check pos duplication
git-svn-id: https://everest.teltel.com:8443/repos/misc/web/nnvmso@2140 a0a5f996-2bb4-401c-8778-395c3c01700f
</commit_message>
<xml_diff>
--- a/war/WEB-INF/views/admin/CSets.xlsx
+++ b/war/WEB-INF/views/admin/CSets.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="144" yWindow="0" windowWidth="12276" windowHeight="11016" tabRatio="622" activeTab="2"/>
+    <workbookView xWindow="144" yWindow="0" windowWidth="12276" windowHeight="11016" tabRatio="622" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Top Level Categories" sheetId="5" r:id="rId1"/>
@@ -3625,10 +3625,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>http://www.maplestage.net/show/流行inHouse</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>http://www.youtube.com/user/diethealth</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -4770,6 +4766,9 @@
   </si>
   <si>
     <t>旅遊休閒</t>
+  </si>
+  <si>
+    <t>http://www.maplestage.net/show/流行in House /</t>
   </si>
 </sst>
 </file>
@@ -5976,7 +5975,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="77" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>1</v>
@@ -6016,7 +6015,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="77" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>1</v>
@@ -6032,7 +6031,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="77" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>1</v>
@@ -6048,7 +6047,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="77" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>1</v>
@@ -6056,7 +6055,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="77" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>1</v>
@@ -6120,7 +6119,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -6143,7 +6142,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>3</v>
@@ -6181,7 +6180,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="77" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>16</v>
@@ -6282,7 +6281,7 @@
         <v>43</v>
       </c>
       <c r="K5" s="77" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>33</v>
@@ -6618,7 +6617,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AR106"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
+      <selection activeCell="AJ13" sqref="AJ13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.95" customHeight="1"/>
   <cols>
@@ -7381,7 +7382,7 @@
         <v>474</v>
       </c>
       <c r="T6" s="20" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="U6" s="48" t="s">
         <v>1047</v>
@@ -7415,10 +7416,10 @@
         <v>688</v>
       </c>
       <c r="AG6" s="38" t="s">
+        <v>1151</v>
+      </c>
+      <c r="AH6" s="61" t="s">
         <v>1152</v>
-      </c>
-      <c r="AH6" s="61" t="s">
-        <v>1153</v>
       </c>
       <c r="AI6" s="31" t="s">
         <v>309</v>
@@ -7643,7 +7644,7 @@
         <v>449</v>
       </c>
       <c r="V8" s="49" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="W8" s="19" t="s">
         <v>638</v>
@@ -7652,10 +7653,10 @@
         <v>639</v>
       </c>
       <c r="AC8" s="16" t="s">
+        <v>1249</v>
+      </c>
+      <c r="AD8" s="17" t="s">
         <v>1250</v>
-      </c>
-      <c r="AD8" s="17" t="s">
-        <v>1251</v>
       </c>
       <c r="AE8" s="19" t="s">
         <v>392</v>
@@ -7780,13 +7781,13 @@
         <v>294</v>
       </c>
       <c r="AD9" s="17" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="AE9" s="73" t="s">
         <v>394</v>
       </c>
       <c r="AF9" s="25" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="AG9" s="31" t="s">
         <v>302</v>
@@ -7802,10 +7803,10 @@
         <v>645</v>
       </c>
       <c r="AK9" s="19" t="s">
+        <v>1295</v>
+      </c>
+      <c r="AL9" s="20" t="s">
         <v>1296</v>
-      </c>
-      <c r="AL9" s="20" t="s">
-        <v>1297</v>
       </c>
       <c r="AM9" s="31" t="s">
         <v>334</v>
@@ -7817,7 +7818,7 @@
         <v>888</v>
       </c>
       <c r="AP9" s="55" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="AQ9" s="56" t="s">
         <v>1037</v>
@@ -7924,7 +7925,7 @@
         <v>528</v>
       </c>
       <c r="AL10" s="49" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="AM10" s="31" t="s">
         <v>330</v>
@@ -7936,7 +7937,7 @@
         <v>456</v>
       </c>
       <c r="AP10" s="20" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="AQ10" s="28" t="s">
         <v>973</v>
@@ -8043,7 +8044,7 @@
         <v>831</v>
       </c>
       <c r="AL11" s="49" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="AM11" s="31" t="s">
         <v>336</v>
@@ -8056,7 +8057,7 @@
         <v>889</v>
       </c>
       <c r="AP11" s="20" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="AQ11" s="28" t="s">
         <v>974</v>
@@ -8161,7 +8162,7 @@
         <v>832</v>
       </c>
       <c r="AL12" s="49" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="AM12" s="15" t="s">
         <v>1062</v>
@@ -8173,13 +8174,13 @@
         <v>890</v>
       </c>
       <c r="AP12" s="20" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="AQ12" s="28" t="s">
         <v>975</v>
       </c>
       <c r="AR12" s="50" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="13" spans="1:44" ht="13.95" customHeight="1">
@@ -8273,13 +8274,13 @@
         <v>209</v>
       </c>
       <c r="AJ13" s="37" t="s">
-        <v>1073</v>
+        <v>1359</v>
       </c>
       <c r="AK13" s="48" t="s">
         <v>833</v>
       </c>
       <c r="AL13" s="49" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="AM13" s="19" t="s">
         <v>532</v>
@@ -8291,13 +8292,13 @@
         <v>891</v>
       </c>
       <c r="AP13" s="20" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="AQ13" s="28" t="s">
         <v>976</v>
       </c>
       <c r="AR13" s="50" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="14" spans="1:44" ht="13.95" customHeight="1">
@@ -8324,25 +8325,25 @@
         <v>819</v>
       </c>
       <c r="H14" s="20" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="I14" s="31" t="s">
         <v>108</v>
       </c>
       <c r="J14" s="39" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="K14" s="36" t="s">
         <v>156</v>
       </c>
       <c r="L14" s="37" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="M14" s="36" t="s">
         <v>247</v>
       </c>
       <c r="N14" s="37" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="O14" s="43" t="s">
         <v>262</v>
@@ -8355,7 +8356,7 @@
         <v>843</v>
       </c>
       <c r="R14" s="25" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="S14" s="19" t="s">
         <v>60</v>
@@ -8398,7 +8399,7 @@
         <v>834</v>
       </c>
       <c r="AL14" s="49" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="AM14" s="52" t="s">
         <v>653</v>
@@ -8410,13 +8411,13 @@
         <v>892</v>
       </c>
       <c r="AP14" s="20" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="AQ14" s="28" t="s">
         <v>977</v>
       </c>
       <c r="AR14" s="50" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="15" spans="1:44" ht="13.95" customHeight="1">
@@ -8468,7 +8469,7 @@
         <v>844</v>
       </c>
       <c r="R15" s="25" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="S15" s="19" t="s">
         <v>1056</v>
@@ -8486,7 +8487,7 @@
         <v>507</v>
       </c>
       <c r="AD15" s="25" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="AE15" s="19" t="s">
         <v>697</v>
@@ -8498,7 +8499,7 @@
         <v>164</v>
       </c>
       <c r="AH15" s="37" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="AI15" s="19" t="s">
         <v>468</v>
@@ -8510,7 +8511,7 @@
         <v>835</v>
       </c>
       <c r="AL15" s="49" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="AM15" s="19" t="s">
         <v>533</v>
@@ -8522,13 +8523,13 @@
         <v>893</v>
       </c>
       <c r="AP15" s="20" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="AQ15" s="21" t="s">
         <v>978</v>
       </c>
       <c r="AR15" s="24" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="16" spans="1:44" ht="13.95" customHeight="1">
@@ -8550,7 +8551,7 @@
         <v>440</v>
       </c>
       <c r="H16" s="20" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="I16" s="31" t="s">
         <v>111</v>
@@ -8580,7 +8581,7 @@
         <v>845</v>
       </c>
       <c r="R16" s="25" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="S16" s="18" t="s">
         <v>293</v>
@@ -8610,7 +8611,7 @@
         <v>212</v>
       </c>
       <c r="AH16" s="37" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="AI16" s="31" t="s">
         <v>372</v>
@@ -8622,7 +8623,7 @@
         <v>836</v>
       </c>
       <c r="AL16" s="49" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="AM16" s="19" t="s">
         <v>534</v>
@@ -8634,7 +8635,7 @@
         <v>979</v>
       </c>
       <c r="AR16" s="24" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="17" spans="1:44" ht="13.95" customHeight="1">
@@ -8654,7 +8655,7 @@
         <v>441</v>
       </c>
       <c r="H17" s="20" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="I17" s="36" t="s">
         <v>242</v>
@@ -8688,10 +8689,10 @@
         <v>847</v>
       </c>
       <c r="S17" s="18" t="s">
+        <v>1081</v>
+      </c>
+      <c r="T17" s="17" t="s">
         <v>1082</v>
-      </c>
-      <c r="T17" s="17" t="s">
-        <v>1083</v>
       </c>
       <c r="U17" s="19" t="s">
         <v>383</v>
@@ -8727,7 +8728,7 @@
         <v>458</v>
       </c>
       <c r="AL17" s="20" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="AM17" s="19" t="s">
         <v>535</v>
@@ -8739,7 +8740,7 @@
         <v>410</v>
       </c>
       <c r="AR17" s="24" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="18" spans="1:44" ht="13.95" customHeight="1">
@@ -8756,7 +8757,7 @@
         <v>672</v>
       </c>
       <c r="G18" s="19" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="H18" s="25" t="s">
         <v>815</v>
@@ -8790,13 +8791,13 @@
         <v>848</v>
       </c>
       <c r="R18" s="25" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="S18" s="18" t="s">
+        <v>1087</v>
+      </c>
+      <c r="T18" s="17" t="s">
         <v>1088</v>
-      </c>
-      <c r="T18" s="17" t="s">
-        <v>1089</v>
       </c>
       <c r="U18" s="19" t="s">
         <v>384</v>
@@ -8817,13 +8818,13 @@
         <v>714</v>
       </c>
       <c r="AG18" s="19" t="s">
+        <v>1274</v>
+      </c>
+      <c r="AH18" s="25" t="s">
         <v>1275</v>
       </c>
-      <c r="AH18" s="25" t="s">
-        <v>1276</v>
-      </c>
       <c r="AI18" s="19" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="AJ18" s="25" t="s">
         <v>868</v>
@@ -8832,7 +8833,7 @@
         <v>460</v>
       </c>
       <c r="AL18" s="20" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="AM18" s="19" t="s">
         <v>536</v>
@@ -8844,7 +8845,7 @@
         <v>980</v>
       </c>
       <c r="AR18" s="24" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="19" spans="1:44" ht="13.95" customHeight="1">
@@ -8864,7 +8865,7 @@
         <v>818</v>
       </c>
       <c r="H19" s="20" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="I19" s="36" t="s">
         <v>241</v>
@@ -8892,10 +8893,10 @@
         <v>http://www.youtube.com/user/lsmovietw</v>
       </c>
       <c r="Q19" s="19" t="s">
+        <v>1103</v>
+      </c>
+      <c r="R19" s="25" t="s">
         <v>1104</v>
-      </c>
-      <c r="R19" s="25" t="s">
-        <v>1105</v>
       </c>
       <c r="S19" s="18" t="s">
         <v>571</v>
@@ -8922,10 +8923,10 @@
         <v>719</v>
       </c>
       <c r="AG19" s="19" t="s">
+        <v>1280</v>
+      </c>
+      <c r="AH19" s="25" t="s">
         <v>1281</v>
-      </c>
-      <c r="AH19" s="25" t="s">
-        <v>1282</v>
       </c>
       <c r="AI19" s="19" t="s">
         <v>859</v>
@@ -8937,19 +8938,19 @@
         <v>450</v>
       </c>
       <c r="AL19" s="20" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="AM19" s="19" t="s">
         <v>537</v>
       </c>
       <c r="AN19" s="20" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="AQ19" s="21" t="s">
         <v>981</v>
       </c>
       <c r="AR19" s="24" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="20" spans="1:44" ht="13.95" customHeight="1">
@@ -8969,7 +8970,7 @@
         <v>821</v>
       </c>
       <c r="H20" s="20" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="I20" s="36" t="s">
         <v>575</v>
@@ -8991,10 +8992,10 @@
         <v>689</v>
       </c>
       <c r="Q20" s="19" t="s">
+        <v>1109</v>
+      </c>
+      <c r="R20" s="25" t="s">
         <v>1110</v>
-      </c>
-      <c r="R20" s="25" t="s">
-        <v>1111</v>
       </c>
       <c r="S20" s="16" t="s">
         <v>90</v>
@@ -9021,10 +9022,10 @@
         <v>725</v>
       </c>
       <c r="AG20" s="19" t="s">
+        <v>1287</v>
+      </c>
+      <c r="AH20" s="25" t="s">
         <v>1288</v>
-      </c>
-      <c r="AH20" s="25" t="s">
-        <v>1289</v>
       </c>
       <c r="AI20" s="19" t="s">
         <v>861</v>
@@ -9036,19 +9037,19 @@
         <v>837</v>
       </c>
       <c r="AL20" s="20" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="AM20" s="19" t="s">
         <v>538</v>
       </c>
       <c r="AN20" s="20" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="AQ20" s="21" t="s">
         <v>982</v>
       </c>
       <c r="AR20" s="24" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="21" spans="1:44" ht="13.95" customHeight="1">
@@ -9056,49 +9057,49 @@
         <v>182</v>
       </c>
       <c r="B21" s="37" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="C21" s="36" t="s">
         <v>166</v>
       </c>
       <c r="D21" s="37" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="G21" s="19" t="s">
         <v>822</v>
       </c>
       <c r="H21" s="20" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="I21" s="36" t="s">
         <v>246</v>
       </c>
       <c r="J21" s="37" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="K21" s="36" t="s">
         <v>151</v>
       </c>
       <c r="L21" s="37" t="s">
+        <v>1120</v>
+      </c>
+      <c r="M21" s="36" t="s">
         <v>1121</v>
       </c>
-      <c r="M21" s="36" t="s">
+      <c r="N21" s="37" t="s">
         <v>1122</v>
       </c>
-      <c r="N21" s="37" t="s">
+      <c r="Q21" s="19" t="s">
         <v>1123</v>
       </c>
-      <c r="Q21" s="19" t="s">
+      <c r="R21" s="25" t="s">
         <v>1124</v>
       </c>
-      <c r="R21" s="25" t="s">
+      <c r="S21" s="16" t="s">
         <v>1125</v>
       </c>
-      <c r="S21" s="16" t="s">
+      <c r="T21" s="17" t="s">
         <v>1126</v>
-      </c>
-      <c r="T21" s="17" t="s">
-        <v>1127</v>
       </c>
       <c r="AC21" s="19" t="s">
         <v>690</v>
@@ -9122,51 +9123,51 @@
         <v>869</v>
       </c>
       <c r="AJ21" s="25" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="AK21" s="19" t="s">
         <v>381</v>
       </c>
       <c r="AL21" s="20" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="AM21" s="19" t="s">
         <v>539</v>
       </c>
       <c r="AN21" s="20" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="AQ21" s="21" t="s">
         <v>983</v>
       </c>
       <c r="AR21" s="24" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="22" spans="1:44" ht="13.95" customHeight="1">
       <c r="A22" s="38" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B22" s="61" t="s">
         <v>1132</v>
-      </c>
-      <c r="B22" s="61" t="s">
-        <v>1133</v>
       </c>
       <c r="C22" s="36" t="s">
         <v>186</v>
       </c>
       <c r="D22" s="37" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="G22" s="19" t="s">
         <v>823</v>
       </c>
       <c r="H22" s="20" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="I22" s="36" t="s">
         <v>240</v>
       </c>
       <c r="J22" s="37" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="K22" s="36" t="s">
         <v>113</v>
@@ -9179,22 +9180,22 @@
         <v>236</v>
       </c>
       <c r="N22" s="37" t="s">
+        <v>1136</v>
+      </c>
+      <c r="Q22" s="19" t="s">
         <v>1137</v>
       </c>
-      <c r="Q22" s="19" t="s">
+      <c r="R22" s="25" t="s">
         <v>1138</v>
-      </c>
-      <c r="R22" s="25" t="s">
-        <v>1139</v>
       </c>
       <c r="S22" s="16" t="s">
         <v>322</v>
       </c>
       <c r="T22" s="17" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="AC22" s="26" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="AD22" s="27" t="s">
         <v>513</v>
@@ -9215,25 +9216,25 @@
         <v>496</v>
       </c>
       <c r="AJ22" s="25" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="AK22" s="19" t="s">
         <v>838</v>
       </c>
       <c r="AL22" s="20" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="AM22" s="19" t="s">
         <v>540</v>
       </c>
       <c r="AN22" s="20" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="AQ22" s="21" t="s">
         <v>984</v>
       </c>
       <c r="AR22" s="24" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="23" spans="1:44" ht="13.95" customHeight="1">
@@ -9241,31 +9242,31 @@
         <v>298</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G23" s="19" t="s">
         <v>824</v>
       </c>
       <c r="H23" s="20" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="I23" s="36" t="s">
         <v>170</v>
       </c>
       <c r="J23" s="37" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="K23" s="36" t="s">
         <v>155</v>
       </c>
       <c r="L23" s="37" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="M23" s="36" t="s">
         <v>185</v>
       </c>
       <c r="N23" s="37" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="Q23" s="31" t="s">
         <v>93</v>
@@ -9274,10 +9275,10 @@
         <v>94</v>
       </c>
       <c r="S23" s="16" t="s">
+        <v>1111</v>
+      </c>
+      <c r="T23" s="17" t="s">
         <v>1112</v>
-      </c>
-      <c r="T23" s="17" t="s">
-        <v>1113</v>
       </c>
       <c r="AC23" s="48" t="s">
         <v>504</v>
@@ -9286,10 +9287,10 @@
         <v>505</v>
       </c>
       <c r="AE23" s="19" t="s">
+        <v>1242</v>
+      </c>
+      <c r="AF23" s="25" t="s">
         <v>1243</v>
-      </c>
-      <c r="AF23" s="25" t="s">
-        <v>1244</v>
       </c>
       <c r="AG23" s="19" t="s">
         <v>482</v>
@@ -9301,60 +9302,60 @@
         <v>863</v>
       </c>
       <c r="AJ23" s="25" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="AK23" s="19" t="s">
         <v>456</v>
       </c>
       <c r="AL23" s="20" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="AM23" s="19" t="s">
         <v>541</v>
       </c>
       <c r="AN23" s="20" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="AQ23" s="21" t="s">
         <v>544</v>
       </c>
       <c r="AR23" s="24" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="24" spans="1:44" ht="13.95" customHeight="1">
       <c r="A24" s="38" t="s">
+        <v>1151</v>
+      </c>
+      <c r="B24" s="61" t="s">
         <v>1152</v>
-      </c>
-      <c r="B24" s="61" t="s">
-        <v>1153</v>
       </c>
       <c r="G24" s="19" t="s">
         <v>825</v>
       </c>
       <c r="H24" s="20" t="s">
+        <v>1153</v>
+      </c>
+      <c r="I24" s="36" t="s">
         <v>1154</v>
       </c>
-      <c r="I24" s="36" t="s">
+      <c r="J24" s="37" t="s">
         <v>1155</v>
-      </c>
-      <c r="J24" s="37" t="s">
-        <v>1156</v>
       </c>
       <c r="K24" s="36" t="s">
         <v>114</v>
       </c>
       <c r="L24" s="37" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="M24" s="36" t="s">
         <v>169</v>
       </c>
       <c r="N24" s="37" t="s">
+        <v>1157</v>
+      </c>
+      <c r="Q24" s="66" t="s">
         <v>1158</v>
-      </c>
-      <c r="Q24" s="66" t="s">
-        <v>1159</v>
       </c>
       <c r="R24" s="20" t="s">
         <v>429</v>
@@ -9370,7 +9371,7 @@
         <v>457</v>
       </c>
       <c r="AD24" s="20" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="AE24" s="52" t="s">
         <v>407</v>
@@ -9388,13 +9389,13 @@
         <v>864</v>
       </c>
       <c r="AJ24" s="25" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="AK24" s="19" t="s">
         <v>384</v>
       </c>
       <c r="AL24" s="20" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="AM24" s="19" t="s">
         <v>542</v>
@@ -9406,7 +9407,7 @@
         <v>985</v>
       </c>
       <c r="AR24" s="24" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="25" spans="1:44" ht="13.95" customHeight="1">
@@ -9417,7 +9418,7 @@
         <v>452</v>
       </c>
       <c r="G25" s="19" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="H25" s="25" t="s">
         <v>826</v>
@@ -9426,26 +9427,26 @@
         <v>218</v>
       </c>
       <c r="J25" s="37" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="K25" s="36" t="s">
         <v>146</v>
       </c>
       <c r="L25" s="37" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="M25" s="47" t="str">
         <f>HYPERLINK("mailto:娛樂@亞洲","娛樂@亞洲")</f>
         <v>娛樂@亞洲</v>
       </c>
       <c r="N25" s="37" t="s">
+        <v>1167</v>
+      </c>
+      <c r="Q25" s="19" t="s">
         <v>1168</v>
       </c>
-      <c r="Q25" s="19" t="s">
+      <c r="R25" s="25" t="s">
         <v>1169</v>
-      </c>
-      <c r="R25" s="25" t="s">
-        <v>1170</v>
       </c>
       <c r="S25" s="33" t="s">
         <v>348</v>
@@ -9457,13 +9458,13 @@
         <v>514</v>
       </c>
       <c r="AD25" s="20" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="AE25" s="48" t="s">
         <v>409</v>
       </c>
       <c r="AF25" s="49" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="AG25" s="19" t="s">
         <v>486</v>
@@ -9475,13 +9476,13 @@
         <v>865</v>
       </c>
       <c r="AJ25" s="25" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="AK25" s="19" t="s">
         <v>457</v>
       </c>
       <c r="AL25" s="20" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="AM25" s="19" t="s">
         <v>544</v>
@@ -9493,12 +9494,12 @@
         <v>986</v>
       </c>
       <c r="AR25" s="24" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="26" spans="1:44" ht="13.95" customHeight="1">
       <c r="A26" s="54" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="B26" s="55" t="s">
         <v>469</v>
@@ -9507,10 +9508,10 @@
         <v>827</v>
       </c>
       <c r="H26" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I26" s="19" t="s">
         <v>1178</v>
-      </c>
-      <c r="I26" s="19" t="s">
-        <v>1179</v>
       </c>
       <c r="J26" s="25" t="s">
         <v>517</v>
@@ -9519,19 +9520,19 @@
         <v>128</v>
       </c>
       <c r="L26" s="37" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="M26" s="36" t="s">
         <v>219</v>
       </c>
       <c r="N26" s="37" t="s">
+        <v>1180</v>
+      </c>
+      <c r="Q26" s="54" t="s">
         <v>1181</v>
       </c>
-      <c r="Q26" s="54" t="s">
+      <c r="R26" s="55" t="s">
         <v>1182</v>
-      </c>
-      <c r="R26" s="55" t="s">
-        <v>1183</v>
       </c>
       <c r="S26" s="31" t="s">
         <v>337</v>
@@ -9541,16 +9542,16 @@
         <v>http://www.youtube.com/user/savedogs2009</v>
       </c>
       <c r="AC26" s="29" t="s">
+        <v>1171</v>
+      </c>
+      <c r="AD26" s="20" t="s">
         <v>1172</v>
-      </c>
-      <c r="AD26" s="20" t="s">
-        <v>1173</v>
       </c>
       <c r="AE26" s="19" t="s">
         <v>410</v>
       </c>
       <c r="AF26" s="20" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="AG26" s="19" t="s">
         <v>488</v>
@@ -9574,15 +9575,15 @@
         <v>987</v>
       </c>
       <c r="AR26" s="24" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="27" spans="1:44" ht="13.95" customHeight="1">
       <c r="A27" s="54" t="s">
+        <v>1187</v>
+      </c>
+      <c r="B27" s="55" t="s">
         <v>1188</v>
-      </c>
-      <c r="B27" s="55" t="s">
-        <v>1189</v>
       </c>
       <c r="G27" s="19" t="s">
         <v>816</v>
@@ -9591,7 +9592,7 @@
         <v>817</v>
       </c>
       <c r="I27" s="52" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="J27" s="25" t="s">
         <v>518</v>
@@ -9609,10 +9610,10 @@
         <v>580</v>
       </c>
       <c r="Q27" s="19" t="s">
+        <v>1190</v>
+      </c>
+      <c r="R27" s="25" t="s">
         <v>1191</v>
-      </c>
-      <c r="R27" s="25" t="s">
-        <v>1192</v>
       </c>
       <c r="S27" s="64" t="s">
         <v>453</v>
@@ -9624,13 +9625,13 @@
         <v>515</v>
       </c>
       <c r="AD27" s="20" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="AE27" s="67" t="s">
         <v>173</v>
       </c>
       <c r="AF27" s="61" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="AG27" s="19" t="s">
         <v>490</v>
@@ -9642,19 +9643,19 @@
         <v>866</v>
       </c>
       <c r="AJ27" s="25" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="AK27" s="48" t="s">
         <v>449</v>
       </c>
       <c r="AL27" s="49" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="AQ27" s="21" t="s">
         <v>988</v>
       </c>
       <c r="AR27" s="24" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="28" spans="1:44" ht="13.95" customHeight="1">
@@ -9689,10 +9690,10 @@
         <v>694</v>
       </c>
       <c r="Q28" s="54" t="s">
+        <v>1196</v>
+      </c>
+      <c r="R28" s="55" t="s">
         <v>1197</v>
-      </c>
-      <c r="R28" s="55" t="s">
-        <v>1198</v>
       </c>
       <c r="S28" s="19" t="s">
         <v>475</v>
@@ -9701,16 +9702,16 @@
         <v>476</v>
       </c>
       <c r="AC28" s="19" t="s">
+        <v>1262</v>
+      </c>
+      <c r="AD28" s="20" t="s">
         <v>1263</v>
-      </c>
-      <c r="AD28" s="20" t="s">
-        <v>1264</v>
       </c>
       <c r="AE28" s="18" t="s">
         <v>293</v>
       </c>
       <c r="AF28" s="17" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="AG28" s="19" t="s">
         <v>492</v>
@@ -9722,7 +9723,7 @@
         <v>867</v>
       </c>
       <c r="AJ28" s="25" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="AK28" s="19" t="s">
         <v>461</v>
@@ -9734,7 +9735,7 @@
         <v>989</v>
       </c>
       <c r="AR28" s="24" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="29" spans="1:44" ht="13.95" customHeight="1">
@@ -9745,7 +9746,7 @@
         <v>342</v>
       </c>
       <c r="G29" s="19" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="H29" s="25" t="s">
         <v>830</v>
@@ -9772,25 +9773,25 @@
         <v>499</v>
       </c>
       <c r="R29" s="55" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="S29" s="19" t="s">
         <v>477</v>
       </c>
       <c r="T29" s="20" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="AC29" s="19" t="s">
+        <v>1271</v>
+      </c>
+      <c r="AD29" s="20" t="s">
         <v>1272</v>
       </c>
-      <c r="AD29" s="20" t="s">
-        <v>1273</v>
-      </c>
       <c r="AE29" s="19" t="s">
+        <v>1285</v>
+      </c>
+      <c r="AF29" s="25" t="s">
         <v>1286</v>
-      </c>
-      <c r="AF29" s="25" t="s">
-        <v>1287</v>
       </c>
       <c r="AG29" s="19" t="s">
         <v>494</v>
@@ -9799,10 +9800,10 @@
         <v>495</v>
       </c>
       <c r="AI29" s="19" t="s">
+        <v>1192</v>
+      </c>
+      <c r="AJ29" s="25" t="s">
         <v>1193</v>
-      </c>
-      <c r="AJ29" s="25" t="s">
-        <v>1194</v>
       </c>
       <c r="AK29" s="19" t="s">
         <v>462</v>
@@ -9819,10 +9820,10 @@
         <v>718</v>
       </c>
       <c r="G30" s="19" t="s">
+        <v>1206</v>
+      </c>
+      <c r="H30" s="25" t="s">
         <v>1207</v>
-      </c>
-      <c r="H30" s="25" t="s">
-        <v>1208</v>
       </c>
       <c r="I30" s="19" t="s">
         <v>721</v>
@@ -9848,19 +9849,19 @@
         <v>381</v>
       </c>
       <c r="T30" s="20" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="AC30" s="19" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AD30" s="25" t="s">
         <v>1233</v>
       </c>
-      <c r="AD30" s="25" t="s">
-        <v>1234</v>
-      </c>
       <c r="AE30" s="16" t="s">
+        <v>1249</v>
+      </c>
+      <c r="AF30" s="17" t="s">
         <v>1250</v>
-      </c>
-      <c r="AF30" s="17" t="s">
-        <v>1251</v>
       </c>
       <c r="AG30" s="19" t="s">
         <v>762</v>
@@ -9869,18 +9870,18 @@
         <v>763</v>
       </c>
       <c r="AI30" s="19" t="s">
+        <v>1184</v>
+      </c>
+      <c r="AJ30" s="25" t="s">
         <v>1185</v>
-      </c>
-      <c r="AJ30" s="25" t="s">
-        <v>1186</v>
       </c>
     </row>
     <row r="31" spans="1:44" ht="13.95" customHeight="1">
       <c r="G31" s="19" t="s">
+        <v>1211</v>
+      </c>
+      <c r="H31" s="25" t="s">
         <v>1212</v>
-      </c>
-      <c r="H31" s="25" t="s">
-        <v>1213</v>
       </c>
       <c r="I31" s="19" t="s">
         <v>520</v>
@@ -9925,7 +9926,7 @@
         <v>875</v>
       </c>
       <c r="AJ31" s="49" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="32" spans="1:44" ht="13.95" customHeight="1">
@@ -9935,7 +9936,7 @@
         <v>435</v>
       </c>
       <c r="H32" s="20" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="I32" s="19" t="s">
         <v>733</v>
@@ -9992,7 +9993,7 @@
         <v>437</v>
       </c>
       <c r="I33" s="19" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="J33" s="25" t="s">
         <v>521</v>
@@ -10042,10 +10043,10 @@
     </row>
     <row r="34" spans="1:38" ht="13.95" customHeight="1">
       <c r="G34" s="19" t="s">
+        <v>1223</v>
+      </c>
+      <c r="H34" s="20" t="s">
         <v>1224</v>
-      </c>
-      <c r="H34" s="20" t="s">
-        <v>1225</v>
       </c>
       <c r="I34" s="23" t="s">
         <v>908</v>
@@ -10068,10 +10069,10 @@
       <c r="Q34" s="19"/>
       <c r="R34" s="25"/>
       <c r="S34" s="19" t="s">
+        <v>1218</v>
+      </c>
+      <c r="T34" s="20" t="s">
         <v>1219</v>
-      </c>
-      <c r="T34" s="20" t="s">
-        <v>1220</v>
       </c>
       <c r="AC34" s="19"/>
       <c r="AD34" s="25"/>
@@ -10091,12 +10092,12 @@
         <v>880</v>
       </c>
       <c r="AJ34" s="20" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="35" spans="1:38" ht="13.95" customHeight="1">
       <c r="G35" s="66" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="H35" s="20" t="s">
         <v>430</v>
@@ -10105,7 +10106,7 @@
         <v>920</v>
       </c>
       <c r="J35" s="24" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="K35" s="36" t="s">
         <v>116</v>
@@ -10125,7 +10126,7 @@
         <v>514</v>
       </c>
       <c r="T35" s="20" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="AC35" s="26"/>
       <c r="AD35" s="27"/>
@@ -10142,10 +10143,10 @@
         <v>804</v>
       </c>
       <c r="AI35" s="19" t="s">
+        <v>1220</v>
+      </c>
+      <c r="AJ35" s="25" t="s">
         <v>1221</v>
-      </c>
-      <c r="AJ35" s="25" t="s">
-        <v>1222</v>
       </c>
     </row>
     <row r="36" spans="1:38" ht="13.95" customHeight="1">
@@ -10155,31 +10156,31 @@
         <v>95</v>
       </c>
       <c r="H36" s="17" t="s">
+        <v>1235</v>
+      </c>
+      <c r="I36" s="71" t="s">
         <v>1236</v>
       </c>
-      <c r="I36" s="71" t="s">
+      <c r="J36" s="70" t="s">
         <v>1237</v>
       </c>
-      <c r="J36" s="70" t="s">
+      <c r="K36" s="36" t="s">
         <v>1238</v>
       </c>
-      <c r="K36" s="36" t="s">
+      <c r="L36" s="37" t="s">
         <v>1239</v>
-      </c>
-      <c r="L36" s="37" t="s">
-        <v>1240</v>
       </c>
       <c r="M36" s="36" t="s">
         <v>167</v>
       </c>
       <c r="N36" s="37" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="S36" s="19" t="s">
         <v>881</v>
       </c>
       <c r="T36" s="20" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="AC36" s="48"/>
       <c r="AD36" s="61"/>
@@ -10190,18 +10191,18 @@
         <v>306</v>
       </c>
       <c r="AI36" s="19" t="s">
+        <v>1226</v>
+      </c>
+      <c r="AJ36" s="25" t="s">
         <v>1227</v>
-      </c>
-      <c r="AJ36" s="25" t="s">
-        <v>1228</v>
       </c>
     </row>
     <row r="37" spans="1:38" ht="13.95" customHeight="1">
       <c r="G37" s="18" t="s">
+        <v>1245</v>
+      </c>
+      <c r="H37" s="17" t="s">
         <v>1246</v>
-      </c>
-      <c r="H37" s="17" t="s">
-        <v>1247</v>
       </c>
       <c r="I37" s="23" t="s">
         <v>874</v>
@@ -10220,13 +10221,13 @@
         <v>248</v>
       </c>
       <c r="N37" s="37" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="S37" s="19" t="s">
         <v>539</v>
       </c>
       <c r="T37" s="20" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="AC37" s="19"/>
       <c r="AD37" s="20"/>
@@ -10240,17 +10241,17 @@
         <v>871</v>
       </c>
       <c r="AJ37" s="20" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="38" spans="1:38" ht="13.95" customHeight="1">
       <c r="A38" s="16"/>
       <c r="B38" s="17"/>
       <c r="G38" s="31" t="s">
+        <v>1252</v>
+      </c>
+      <c r="H38" s="17" t="s">
         <v>1253</v>
-      </c>
-      <c r="H38" s="17" t="s">
-        <v>1254</v>
       </c>
       <c r="I38" s="23" t="s">
         <v>916</v>
@@ -10269,13 +10270,13 @@
         <v>182</v>
       </c>
       <c r="N38" s="37" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="S38" s="19" t="s">
         <v>882</v>
       </c>
       <c r="T38" s="20" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="AC38" s="19"/>
       <c r="AD38" s="20"/>
@@ -10296,28 +10297,28 @@
       <c r="A39" s="16"/>
       <c r="B39" s="17"/>
       <c r="G39" s="16" t="s">
+        <v>1258</v>
+      </c>
+      <c r="H39" s="17" t="s">
         <v>1259</v>
       </c>
-      <c r="H39" s="17" t="s">
-        <v>1260</v>
-      </c>
       <c r="I39" s="52" t="s">
+        <v>1266</v>
+      </c>
+      <c r="J39" s="25" t="s">
         <v>1267</v>
-      </c>
-      <c r="J39" s="25" t="s">
-        <v>1268</v>
       </c>
       <c r="K39" s="36" t="s">
         <v>133</v>
       </c>
       <c r="L39" s="37" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="M39" s="36" t="s">
         <v>234</v>
       </c>
       <c r="N39" s="37" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="S39" s="31" t="s">
         <v>339</v>
@@ -10340,7 +10341,7 @@
       <c r="A40" s="19"/>
       <c r="B40" s="25"/>
       <c r="G40" s="66" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="H40" s="20" t="s">
         <v>429</v>
@@ -10355,13 +10356,13 @@
         <v>143</v>
       </c>
       <c r="L40" s="37" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="M40" s="36" t="s">
         <v>242</v>
       </c>
       <c r="N40" s="37" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="S40" s="31" t="s">
         <v>341</v>
@@ -10384,10 +10385,10 @@
       <c r="A41" s="19"/>
       <c r="B41" s="25"/>
       <c r="G41" s="19" t="s">
+        <v>1168</v>
+      </c>
+      <c r="H41" s="25" t="s">
         <v>1169</v>
-      </c>
-      <c r="H41" s="25" t="s">
-        <v>1170</v>
       </c>
       <c r="I41" s="71" t="s">
         <v>937</v>
@@ -10399,19 +10400,19 @@
         <v>131</v>
       </c>
       <c r="L41" s="37" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="M41" s="36" t="s">
         <v>246</v>
       </c>
       <c r="N41" s="37" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="S41" s="31" t="s">
         <v>343</v>
       </c>
       <c r="T41" s="39" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="AG41" s="36" t="s">
         <v>226</v>
@@ -10426,13 +10427,13 @@
       <c r="A42" s="19"/>
       <c r="B42" s="25"/>
       <c r="G42" s="54" t="s">
+        <v>1181</v>
+      </c>
+      <c r="H42" s="55" t="s">
         <v>1182</v>
       </c>
-      <c r="H42" s="55" t="s">
-        <v>1183</v>
-      </c>
       <c r="I42" s="54" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="J42" s="25" t="s">
         <v>516</v>
@@ -10441,13 +10442,13 @@
         <v>121</v>
       </c>
       <c r="L42" s="37" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="M42" s="36" t="s">
         <v>206</v>
       </c>
       <c r="N42" s="37" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="AG42" s="36" t="s">
         <v>239</v>
@@ -10460,28 +10461,28 @@
       <c r="A43" s="19"/>
       <c r="B43" s="25"/>
       <c r="G43" s="19" t="s">
+        <v>1289</v>
+      </c>
+      <c r="H43" s="25" t="s">
         <v>1290</v>
       </c>
-      <c r="H43" s="25" t="s">
-        <v>1291</v>
-      </c>
       <c r="I43" s="54" t="s">
+        <v>1297</v>
+      </c>
+      <c r="J43" s="25" t="s">
         <v>1298</v>
-      </c>
-      <c r="J43" s="25" t="s">
-        <v>1299</v>
       </c>
       <c r="K43" s="36" t="s">
         <v>161</v>
       </c>
       <c r="L43" s="37" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="M43" s="36" t="s">
         <v>162</v>
       </c>
       <c r="N43" s="37" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="AG43" s="36" t="s">
         <v>201</v>
@@ -10534,10 +10535,10 @@
         <v>465</v>
       </c>
       <c r="I45" s="19" t="s">
+        <v>1300</v>
+      </c>
+      <c r="J45" s="25" t="s">
         <v>1301</v>
-      </c>
-      <c r="J45" s="25" t="s">
-        <v>1302</v>
       </c>
       <c r="K45" s="36" t="s">
         <v>153</v>
@@ -10574,7 +10575,7 @@
         <v>522</v>
       </c>
       <c r="J46" s="68" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="K46" s="36" t="s">
         <v>158</v>
@@ -10604,13 +10605,13 @@
         <v>390</v>
       </c>
       <c r="H47" s="25" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="I47" s="67" t="s">
         <v>523</v>
       </c>
       <c r="J47" s="68" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="K47" s="36" t="s">
         <v>159</v>
@@ -10714,7 +10715,7 @@
         <v>947</v>
       </c>
       <c r="J50" s="70" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="K50" s="36" t="s">
         <v>138</v>
@@ -10748,7 +10749,7 @@
         <v>522</v>
       </c>
       <c r="J51" s="70" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="K51" s="36" t="s">
         <v>127</v>
@@ -10783,7 +10784,7 @@
         <v>948</v>
       </c>
       <c r="J52" s="70" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="K52" s="36" t="s">
         <v>132</v>
@@ -10810,7 +10811,7 @@
     </row>
     <row r="53" spans="7:34" ht="13.95" customHeight="1">
       <c r="G53" s="19" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="H53" s="25" t="s">
         <v>92</v>
@@ -10819,7 +10820,7 @@
         <v>949</v>
       </c>
       <c r="J53" s="70" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="K53" s="36" t="s">
         <v>119</v>
@@ -10846,16 +10847,16 @@
     </row>
     <row r="54" spans="7:34" ht="13.95" customHeight="1">
       <c r="G54" s="19" t="s">
+        <v>1305</v>
+      </c>
+      <c r="H54" s="25" t="s">
         <v>1306</v>
-      </c>
-      <c r="H54" s="25" t="s">
-        <v>1307</v>
       </c>
       <c r="I54" s="71" t="s">
         <v>950</v>
       </c>
       <c r="J54" s="70" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="K54" s="33" t="s">
         <v>268</v>
@@ -10892,7 +10893,7 @@
         <v>951</v>
       </c>
       <c r="J55" s="70" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="K55" s="33" t="s">
         <v>269</v>
@@ -10927,7 +10928,7 @@
         <v>952</v>
       </c>
       <c r="J56" s="70" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="K56" s="33" t="s">
         <v>270</v>
@@ -10961,7 +10962,7 @@
         <v>953</v>
       </c>
       <c r="J57" s="70" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="K57" s="33" t="s">
         <v>272</v>
@@ -10995,7 +10996,7 @@
         <v>954</v>
       </c>
       <c r="J58" s="70" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="K58" s="33" t="s">
         <v>274</v>
@@ -11100,7 +11101,7 @@
         <v>523</v>
       </c>
       <c r="J61" s="70" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="K61" s="31" t="s">
         <v>355</v>
@@ -11133,10 +11134,10 @@
         <v>415</v>
       </c>
       <c r="I62" s="19" t="s">
+        <v>1322</v>
+      </c>
+      <c r="J62" s="25" t="s">
         <v>1323</v>
-      </c>
-      <c r="J62" s="25" t="s">
-        <v>1324</v>
       </c>
       <c r="M62" s="36" t="s">
         <v>240</v>
@@ -11186,10 +11187,10 @@
         <v>418</v>
       </c>
       <c r="H64" s="49" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="I64" s="23" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="J64" s="24" t="s">
         <v>903</v>
@@ -11214,7 +11215,7 @@
         <v>419</v>
       </c>
       <c r="H65" s="68" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="I65" s="23" t="s">
         <v>906</v>
@@ -11242,7 +11243,7 @@
         <v>420</v>
       </c>
       <c r="H66" s="68" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="I66" s="23" t="s">
         <v>913</v>
@@ -11270,7 +11271,7 @@
         <v>421</v>
       </c>
       <c r="H67" s="68" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="I67" s="67" t="s">
         <v>524</v>
@@ -11320,7 +11321,7 @@
         <v>424</v>
       </c>
       <c r="H69" s="68" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="I69" s="23" t="s">
         <v>909</v>
@@ -11403,7 +11404,7 @@
         <v>921</v>
       </c>
       <c r="J73" s="70" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="74" spans="7:34" ht="13.95" customHeight="1">
@@ -11431,7 +11432,7 @@
         <v>924</v>
       </c>
       <c r="J75" s="70" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="76" spans="7:34" ht="13.95" customHeight="1">
@@ -11445,7 +11446,7 @@
         <v>925</v>
       </c>
       <c r="J76" s="70" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="77" spans="7:34" ht="13.95" customHeight="1">
@@ -11459,7 +11460,7 @@
         <v>926</v>
       </c>
       <c r="J77" s="70" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="78" spans="7:34" ht="13.95" customHeight="1">
@@ -11473,7 +11474,7 @@
         <v>927</v>
       </c>
       <c r="J78" s="70" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="M78" s="36"/>
       <c r="N78" s="37"/>
@@ -11483,7 +11484,7 @@
         <v>928</v>
       </c>
       <c r="J79" s="70" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="M79" s="36"/>
       <c r="N79" s="37"/>
@@ -11493,7 +11494,7 @@
         <v>929</v>
       </c>
       <c r="J80" s="70" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="M80" s="36"/>
       <c r="N80" s="37"/>
@@ -11503,7 +11504,7 @@
         <v>930</v>
       </c>
       <c r="J81" s="70" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="M81" s="36"/>
       <c r="N81" s="37"/>
@@ -11513,7 +11514,7 @@
         <v>931</v>
       </c>
       <c r="J82" s="70" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="M82" s="36"/>
       <c r="N82" s="37"/>
@@ -11523,7 +11524,7 @@
         <v>932</v>
       </c>
       <c r="J83" s="70" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="M83" s="36"/>
       <c r="N83" s="37"/>
@@ -11533,7 +11534,7 @@
         <v>933</v>
       </c>
       <c r="J84" s="70" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="M84" s="36"/>
       <c r="N84" s="37"/>
@@ -11543,7 +11544,7 @@
         <v>934</v>
       </c>
       <c r="J85" s="70" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="M85" s="36"/>
       <c r="N85" s="37"/>
@@ -11613,7 +11614,7 @@
         <v>959</v>
       </c>
       <c r="J92" s="70" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="M92" s="36"/>
       <c r="N92" s="37"/>
@@ -11623,7 +11624,7 @@
         <v>960</v>
       </c>
       <c r="J93" s="70" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="M93" s="47"/>
       <c r="N93" s="37"/>
@@ -11633,7 +11634,7 @@
         <v>961</v>
       </c>
       <c r="J94" s="70" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="M94" s="36"/>
       <c r="N94" s="37"/>
@@ -11643,7 +11644,7 @@
         <v>856</v>
       </c>
       <c r="J95" s="70" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="M95" s="36"/>
       <c r="N95" s="37"/>
@@ -11653,7 +11654,7 @@
         <v>962</v>
       </c>
       <c r="J96" s="70" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="M96" s="36"/>
       <c r="N96" s="37"/>
@@ -11663,7 +11664,7 @@
         <v>963</v>
       </c>
       <c r="J97" s="70" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="M97" s="36"/>
       <c r="N97" s="37"/>
@@ -11673,7 +11674,7 @@
         <v>964</v>
       </c>
       <c r="J98" s="70" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="M98" s="36"/>
       <c r="N98" s="37"/>
@@ -11683,7 +11684,7 @@
         <v>966</v>
       </c>
       <c r="J99" s="70" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="M99" s="36"/>
       <c r="N99" s="37"/>
@@ -11693,7 +11694,7 @@
         <v>965</v>
       </c>
       <c r="J100" s="70" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="M100" s="36"/>
       <c r="N100" s="37"/>
@@ -11713,7 +11714,7 @@
         <v>967</v>
       </c>
       <c r="J102" s="70" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="M102" s="36"/>
       <c r="N102" s="37"/>
@@ -11723,7 +11724,7 @@
         <v>968</v>
       </c>
       <c r="J103" s="70" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="M103" s="36"/>
       <c r="N103" s="37"/>
@@ -11733,17 +11734,17 @@
         <v>969</v>
       </c>
       <c r="J104" s="24" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="M104" s="36"/>
       <c r="N104" s="37"/>
     </row>
     <row r="105" spans="9:14" ht="13.95" customHeight="1">
       <c r="I105" s="54" t="s">
+        <v>1350</v>
+      </c>
+      <c r="J105" s="25" t="s">
         <v>1351</v>
-      </c>
-      <c r="J105" s="25" t="s">
-        <v>1352</v>
       </c>
     </row>
     <row r="106" spans="9:14" ht="13.95" customHeight="1">
@@ -11832,517 +11833,516 @@
     <hyperlink ref="F9" r:id="rId72"/>
     <hyperlink ref="AJ11" r:id="rId73"/>
     <hyperlink ref="AJ12" r:id="rId74"/>
-    <hyperlink ref="AJ13" r:id="rId75"/>
-    <hyperlink ref="AH38" r:id="rId76"/>
-    <hyperlink ref="X6" r:id="rId77"/>
-    <hyperlink ref="AH37" r:id="rId78"/>
-    <hyperlink ref="D17" r:id="rId79"/>
-    <hyperlink ref="D18" r:id="rId80"/>
-    <hyperlink ref="D19" r:id="rId81"/>
-    <hyperlink ref="D20" r:id="rId82"/>
-    <hyperlink ref="D21" r:id="rId83"/>
-    <hyperlink ref="D22" r:id="rId84"/>
-    <hyperlink ref="N2" r:id="rId85"/>
-    <hyperlink ref="N3" r:id="rId86"/>
-    <hyperlink ref="N4" r:id="rId87"/>
-    <hyperlink ref="N6" r:id="rId88"/>
-    <hyperlink ref="N10" r:id="rId89"/>
-    <hyperlink ref="N11" r:id="rId90"/>
-    <hyperlink ref="N12" r:id="rId91"/>
-    <hyperlink ref="N13" r:id="rId92"/>
-    <hyperlink ref="N14" r:id="rId93"/>
-    <hyperlink ref="N28" r:id="rId94"/>
-    <hyperlink ref="N20" r:id="rId95"/>
-    <hyperlink ref="N21" r:id="rId96"/>
-    <hyperlink ref="N22" r:id="rId97"/>
-    <hyperlink ref="N24" r:id="rId98"/>
-    <hyperlink ref="N25" r:id="rId99"/>
-    <hyperlink ref="N26" r:id="rId100"/>
-    <hyperlink ref="N27" r:id="rId101"/>
-    <hyperlink ref="N34" r:id="rId102"/>
-    <hyperlink ref="N39" r:id="rId103"/>
-    <hyperlink ref="N36" r:id="rId104"/>
-    <hyperlink ref="N37" r:id="rId105"/>
-    <hyperlink ref="N38" r:id="rId106"/>
-    <hyperlink ref="N16" r:id="rId107"/>
-    <hyperlink ref="N17" r:id="rId108"/>
-    <hyperlink ref="N18" r:id="rId109"/>
-    <hyperlink ref="N23" r:id="rId110"/>
-    <hyperlink ref="N19" r:id="rId111"/>
-    <hyperlink ref="N7" r:id="rId112"/>
-    <hyperlink ref="N8" r:id="rId113"/>
-    <hyperlink ref="N15" r:id="rId114"/>
-    <hyperlink ref="N44" r:id="rId115"/>
-    <hyperlink ref="N29" r:id="rId116"/>
-    <hyperlink ref="N30" r:id="rId117"/>
-    <hyperlink ref="N32" r:id="rId118"/>
-    <hyperlink ref="N33" r:id="rId119"/>
-    <hyperlink ref="N35" r:id="rId120"/>
-    <hyperlink ref="N40" r:id="rId121"/>
-    <hyperlink ref="N41" r:id="rId122"/>
-    <hyperlink ref="N45" r:id="rId123"/>
-    <hyperlink ref="N46" r:id="rId124"/>
-    <hyperlink ref="N42" r:id="rId125"/>
-    <hyperlink ref="N43" r:id="rId126"/>
-    <hyperlink ref="N47" r:id="rId127"/>
-    <hyperlink ref="N48" r:id="rId128"/>
-    <hyperlink ref="N49" r:id="rId129"/>
-    <hyperlink ref="N50" r:id="rId130"/>
-    <hyperlink ref="N51" r:id="rId131"/>
-    <hyperlink ref="N53" r:id="rId132"/>
-    <hyperlink ref="N54" r:id="rId133"/>
-    <hyperlink ref="N55" r:id="rId134"/>
-    <hyperlink ref="N56" r:id="rId135"/>
-    <hyperlink ref="N57" r:id="rId136"/>
-    <hyperlink ref="N58" r:id="rId137"/>
-    <hyperlink ref="N59" r:id="rId138"/>
-    <hyperlink ref="N60" r:id="rId139"/>
-    <hyperlink ref="N62" r:id="rId140"/>
-    <hyperlink ref="N63" r:id="rId141"/>
-    <hyperlink ref="N64" r:id="rId142"/>
-    <hyperlink ref="N65" r:id="rId143"/>
-    <hyperlink ref="N66" r:id="rId144"/>
-    <hyperlink ref="N69" r:id="rId145"/>
-    <hyperlink ref="N67" r:id="rId146"/>
-    <hyperlink ref="N68" r:id="rId147"/>
-    <hyperlink ref="N70" r:id="rId148"/>
-    <hyperlink ref="B19" r:id="rId149"/>
-    <hyperlink ref="B20" r:id="rId150"/>
-    <hyperlink ref="B21" r:id="rId151"/>
-    <hyperlink ref="V15" r:id="rId152"/>
-    <hyperlink ref="V10" r:id="rId153"/>
-    <hyperlink ref="V11" r:id="rId154"/>
-    <hyperlink ref="V16" r:id="rId155"/>
-    <hyperlink ref="V18" r:id="rId156"/>
-    <hyperlink ref="V17" r:id="rId157"/>
-    <hyperlink ref="V19" r:id="rId158"/>
-    <hyperlink ref="H3" r:id="rId159"/>
-    <hyperlink ref="H8" r:id="rId160"/>
-    <hyperlink ref="H11" r:id="rId161"/>
-    <hyperlink ref="H47" r:id="rId162"/>
-    <hyperlink ref="H12" r:id="rId163"/>
-    <hyperlink ref="H31" r:id="rId164"/>
-    <hyperlink ref="H34" r:id="rId165"/>
-    <hyperlink ref="H36" r:id="rId166"/>
-    <hyperlink ref="H37" r:id="rId167"/>
-    <hyperlink ref="H39" r:id="rId168"/>
-    <hyperlink ref="H6" r:id="rId169"/>
-    <hyperlink ref="H38" r:id="rId170"/>
-    <hyperlink ref="H43" r:id="rId171"/>
-    <hyperlink ref="H42" r:id="rId172"/>
-    <hyperlink ref="H41" r:id="rId173"/>
-    <hyperlink ref="H54" r:id="rId174"/>
-    <hyperlink ref="H2" r:id="rId175"/>
-    <hyperlink ref="H7" r:id="rId176"/>
-    <hyperlink ref="H4" r:id="rId177"/>
-    <hyperlink ref="AF27" r:id="rId178"/>
-    <hyperlink ref="AF34" r:id="rId179"/>
-    <hyperlink ref="AF35" r:id="rId180"/>
-    <hyperlink ref="AF5" r:id="rId181"/>
-    <hyperlink ref="AF32" r:id="rId182"/>
-    <hyperlink ref="AF33" r:id="rId183"/>
-    <hyperlink ref="AF28" r:id="rId184"/>
-    <hyperlink ref="AF6" r:id="rId185"/>
-    <hyperlink ref="AF3" r:id="rId186"/>
-    <hyperlink ref="AF4" r:id="rId187"/>
-    <hyperlink ref="AF2" r:id="rId188"/>
-    <hyperlink ref="AF30" r:id="rId189"/>
-    <hyperlink ref="AF8" r:id="rId190"/>
-    <hyperlink ref="AF7" r:id="rId191"/>
-    <hyperlink ref="AF29" r:id="rId192"/>
-    <hyperlink ref="AF20" r:id="rId193"/>
-    <hyperlink ref="AF9" r:id="rId194"/>
-    <hyperlink ref="AF11" r:id="rId195"/>
-    <hyperlink ref="AF12" r:id="rId196"/>
-    <hyperlink ref="AF13" r:id="rId197"/>
-    <hyperlink ref="AF14" r:id="rId198"/>
-    <hyperlink ref="AF15" r:id="rId199"/>
-    <hyperlink ref="AF16" r:id="rId200"/>
-    <hyperlink ref="AF17" r:id="rId201"/>
-    <hyperlink ref="AF21" r:id="rId202"/>
-    <hyperlink ref="AF23" r:id="rId203"/>
-    <hyperlink ref="AF18" r:id="rId204"/>
-    <hyperlink ref="AF24" r:id="rId205"/>
-    <hyperlink ref="AF19" r:id="rId206"/>
-    <hyperlink ref="AF22" r:id="rId207"/>
-    <hyperlink ref="AF25" r:id="rId208"/>
-    <hyperlink ref="AF26" r:id="rId209"/>
-    <hyperlink ref="AF10" r:id="rId210"/>
-    <hyperlink ref="AF31" r:id="rId211"/>
-    <hyperlink ref="H68" r:id="rId212"/>
-    <hyperlink ref="H62" r:id="rId213"/>
-    <hyperlink ref="H61" r:id="rId214"/>
-    <hyperlink ref="H73" r:id="rId215"/>
-    <hyperlink ref="H59" r:id="rId216"/>
-    <hyperlink ref="H60" r:id="rId217"/>
-    <hyperlink ref="H65" r:id="rId218"/>
-    <hyperlink ref="H67" r:id="rId219"/>
-    <hyperlink ref="H66" r:id="rId220"/>
-    <hyperlink ref="H69" r:id="rId221"/>
-    <hyperlink ref="H64" r:id="rId222"/>
-    <hyperlink ref="H70" r:id="rId223"/>
-    <hyperlink ref="H72" r:id="rId224"/>
-    <hyperlink ref="H63" r:id="rId225"/>
-    <hyperlink ref="H71" r:id="rId226"/>
-    <hyperlink ref="H51" r:id="rId227"/>
-    <hyperlink ref="H46" r:id="rId228"/>
-    <hyperlink ref="H40" r:id="rId229"/>
-    <hyperlink ref="H76" r:id="rId230"/>
-    <hyperlink ref="H32" r:id="rId231"/>
-    <hyperlink ref="H15" r:id="rId232"/>
-    <hyperlink ref="H16" r:id="rId233"/>
-    <hyperlink ref="H17" r:id="rId234"/>
-    <hyperlink ref="H5" r:id="rId235"/>
-    <hyperlink ref="H10" r:id="rId236"/>
-    <hyperlink ref="H56" r:id="rId237"/>
-    <hyperlink ref="H35" r:id="rId238"/>
-    <hyperlink ref="H77" r:id="rId239"/>
-    <hyperlink ref="H78" r:id="rId240"/>
-    <hyperlink ref="H57" r:id="rId241"/>
-    <hyperlink ref="F12" r:id="rId242"/>
-    <hyperlink ref="B25" r:id="rId243"/>
-    <hyperlink ref="AD10" r:id="rId244"/>
-    <hyperlink ref="F13" r:id="rId245"/>
-    <hyperlink ref="AD11" r:id="rId246"/>
-    <hyperlink ref="AD12" r:id="rId247"/>
-    <hyperlink ref="F14" r:id="rId248"/>
-    <hyperlink ref="H58" r:id="rId249"/>
-    <hyperlink ref="V2" r:id="rId250"/>
-    <hyperlink ref="V3" r:id="rId251"/>
-    <hyperlink ref="AL27" r:id="rId252"/>
-    <hyperlink ref="AL28" r:id="rId253"/>
-    <hyperlink ref="AL29" r:id="rId254"/>
-    <hyperlink ref="X9" r:id="rId255"/>
-    <hyperlink ref="X8" r:id="rId256"/>
-    <hyperlink ref="X7" r:id="rId257"/>
-    <hyperlink ref="H44" r:id="rId258"/>
-    <hyperlink ref="R9" r:id="rId259" display="http://www.youtube.com/user/motorstelevision"/>
-    <hyperlink ref="B26" r:id="rId260"/>
-    <hyperlink ref="B27" r:id="rId261"/>
-    <hyperlink ref="H52" r:id="rId262"/>
-    <hyperlink ref="H49" r:id="rId263"/>
-    <hyperlink ref="H50" r:id="rId264"/>
-    <hyperlink ref="AH18" r:id="rId265"/>
-    <hyperlink ref="AH19" r:id="rId266"/>
-    <hyperlink ref="AH20" r:id="rId267"/>
-    <hyperlink ref="AH28" r:id="rId268"/>
-    <hyperlink ref="AH29" r:id="rId269"/>
-    <hyperlink ref="AH30" r:id="rId270"/>
-    <hyperlink ref="AH31" r:id="rId271"/>
-    <hyperlink ref="AH32" r:id="rId272"/>
-    <hyperlink ref="AH33" r:id="rId273"/>
-    <hyperlink ref="AH10" r:id="rId274"/>
-    <hyperlink ref="AH11" r:id="rId275"/>
-    <hyperlink ref="AH54" r:id="rId276"/>
-    <hyperlink ref="AH66" r:id="rId277"/>
-    <hyperlink ref="AH55" r:id="rId278"/>
-    <hyperlink ref="AH56" r:id="rId279"/>
-    <hyperlink ref="AH67" r:id="rId280"/>
-    <hyperlink ref="AH59" r:id="rId281"/>
-    <hyperlink ref="AH64" r:id="rId282"/>
-    <hyperlink ref="AH34" r:id="rId283"/>
-    <hyperlink ref="AH35" r:id="rId284"/>
-    <hyperlink ref="X2" r:id="rId285"/>
-    <hyperlink ref="X3" r:id="rId286"/>
-    <hyperlink ref="AD15" r:id="rId287"/>
-    <hyperlink ref="AD16" r:id="rId288"/>
-    <hyperlink ref="AD17" r:id="rId289"/>
-    <hyperlink ref="AD18" r:id="rId290"/>
-    <hyperlink ref="AD19" r:id="rId291"/>
-    <hyperlink ref="AD20" r:id="rId292"/>
-    <hyperlink ref="AD21" r:id="rId293"/>
-    <hyperlink ref="AD23" r:id="rId294"/>
-    <hyperlink ref="AD13" r:id="rId295"/>
-    <hyperlink ref="AD24" r:id="rId296"/>
-    <hyperlink ref="AD14" r:id="rId297"/>
-    <hyperlink ref="AD25" r:id="rId298"/>
-    <hyperlink ref="AD27" r:id="rId299"/>
-    <hyperlink ref="AD26" r:id="rId300"/>
-    <hyperlink ref="AH12" r:id="rId301"/>
-    <hyperlink ref="AH60" r:id="rId302"/>
-    <hyperlink ref="AH63" r:id="rId303"/>
-    <hyperlink ref="AH57" r:id="rId304"/>
-    <hyperlink ref="AH58" r:id="rId305"/>
-    <hyperlink ref="AH62" r:id="rId306"/>
-    <hyperlink ref="AH61" r:id="rId307"/>
-    <hyperlink ref="AH65" r:id="rId308"/>
-    <hyperlink ref="AN12" r:id="rId309"/>
-    <hyperlink ref="AN14" r:id="rId310"/>
-    <hyperlink ref="AN24" r:id="rId311"/>
-    <hyperlink ref="AN19" r:id="rId312"/>
-    <hyperlink ref="AN13" r:id="rId313"/>
-    <hyperlink ref="AN15" r:id="rId314"/>
-    <hyperlink ref="AN17" r:id="rId315"/>
-    <hyperlink ref="AN16" r:id="rId316"/>
-    <hyperlink ref="AN18" r:id="rId317"/>
-    <hyperlink ref="AN20" r:id="rId318"/>
-    <hyperlink ref="AN21" r:id="rId319"/>
-    <hyperlink ref="AN22" r:id="rId320"/>
-    <hyperlink ref="AN23" r:id="rId321"/>
-    <hyperlink ref="AN25" r:id="rId322"/>
-    <hyperlink ref="AD28" r:id="rId323"/>
-    <hyperlink ref="AD29" r:id="rId324"/>
-    <hyperlink ref="H9" r:id="rId325"/>
-    <hyperlink ref="H29" r:id="rId326"/>
-    <hyperlink ref="H30" r:id="rId327"/>
-    <hyperlink ref="H19" r:id="rId328"/>
-    <hyperlink ref="H14" r:id="rId329"/>
-    <hyperlink ref="H21" r:id="rId330"/>
-    <hyperlink ref="H20" r:id="rId331"/>
-    <hyperlink ref="H13" r:id="rId332"/>
-    <hyperlink ref="H22" r:id="rId333"/>
-    <hyperlink ref="H23" r:id="rId334"/>
-    <hyperlink ref="H24" r:id="rId335"/>
-    <hyperlink ref="AL10" r:id="rId336"/>
-    <hyperlink ref="AL11" r:id="rId337"/>
-    <hyperlink ref="AL19" r:id="rId338"/>
-    <hyperlink ref="AL12" r:id="rId339"/>
-    <hyperlink ref="AL21" r:id="rId340"/>
-    <hyperlink ref="AL13" r:id="rId341"/>
-    <hyperlink ref="AL22" r:id="rId342"/>
-    <hyperlink ref="AL14" r:id="rId343"/>
-    <hyperlink ref="AL23" r:id="rId344"/>
-    <hyperlink ref="AL15" r:id="rId345"/>
-    <hyperlink ref="AL16" r:id="rId346"/>
-    <hyperlink ref="AL17" r:id="rId347"/>
-    <hyperlink ref="AL18" r:id="rId348"/>
-    <hyperlink ref="AL24" r:id="rId349"/>
-    <hyperlink ref="AL25" r:id="rId350"/>
-    <hyperlink ref="AL20" r:id="rId351"/>
-    <hyperlink ref="AL9" r:id="rId352"/>
-    <hyperlink ref="R23" r:id="rId353" display="http://www.youtube.com/user/MINI"/>
-    <hyperlink ref="R30" r:id="rId354" display="http://www.youtube.com/user/motousa"/>
-    <hyperlink ref="R32" r:id="rId355" display="http://www.youtube.com/user/autocar"/>
-    <hyperlink ref="R33" r:id="rId356" display="http://www.youtube.com/user/TopGear"/>
-    <hyperlink ref="R34" r:id="rId357" display="http://www.youtube.com/user/motorstelevision"/>
-    <hyperlink ref="R37" r:id="rId358" display="http://www.youtube.com/user/militarychannel"/>
-    <hyperlink ref="R38" r:id="rId359" display="http://www.youtube.com/user/carshowclassic"/>
-    <hyperlink ref="R39" r:id="rId360" display="http://www.youtube.com/user/Motorscouk"/>
-    <hyperlink ref="R40" r:id="rId361" display="http://www.youtube.com/user/EmiratesExperience"/>
-    <hyperlink ref="R42" r:id="rId362" display="http://www.youtube.com/user/rockitoutblog"/>
-    <hyperlink ref="R43" r:id="rId363" display="http://www.youtube.com/user/musiciansinstitute"/>
-    <hyperlink ref="R44" r:id="rId364" display="http://www.youtube.com/user/GuitarCenterTV"/>
-    <hyperlink ref="R46" r:id="rId365" display="http://www.youtube.com/user/TylerWardMusic"/>
-    <hyperlink ref="AJ17" r:id="rId366"/>
-    <hyperlink ref="AJ23" r:id="rId367"/>
-    <hyperlink ref="AJ24" r:id="rId368"/>
-    <hyperlink ref="AJ25" r:id="rId369"/>
-    <hyperlink ref="AJ26" r:id="rId370"/>
-    <hyperlink ref="AJ27" r:id="rId371"/>
-    <hyperlink ref="AJ22" r:id="rId372"/>
-    <hyperlink ref="AJ30" r:id="rId373"/>
-    <hyperlink ref="AJ29" r:id="rId374"/>
-    <hyperlink ref="AJ28" r:id="rId375"/>
-    <hyperlink ref="AJ18" r:id="rId376"/>
-    <hyperlink ref="AJ21" r:id="rId377"/>
-    <hyperlink ref="AJ35" r:id="rId378"/>
-    <hyperlink ref="AJ36" r:id="rId379"/>
-    <hyperlink ref="AD30" r:id="rId380"/>
-    <hyperlink ref="AJ32" r:id="rId381"/>
-    <hyperlink ref="AJ33" r:id="rId382"/>
-    <hyperlink ref="AJ31" r:id="rId383"/>
-    <hyperlink ref="AJ34" r:id="rId384"/>
-    <hyperlink ref="AJ37" r:id="rId385"/>
-    <hyperlink ref="AP2" r:id="rId386"/>
-    <hyperlink ref="AP4" r:id="rId387"/>
-    <hyperlink ref="AP5" r:id="rId388"/>
-    <hyperlink ref="AP6" r:id="rId389"/>
-    <hyperlink ref="AP9" r:id="rId390"/>
-    <hyperlink ref="AP10" r:id="rId391"/>
-    <hyperlink ref="AP12" r:id="rId392"/>
-    <hyperlink ref="AP11" r:id="rId393"/>
-    <hyperlink ref="AP13" r:id="rId394"/>
-    <hyperlink ref="AP15" r:id="rId395"/>
-    <hyperlink ref="AP14" r:id="rId396"/>
-    <hyperlink ref="B24" r:id="rId397"/>
-    <hyperlink ref="B22" r:id="rId398"/>
-    <hyperlink ref="AR2" r:id="rId399"/>
-    <hyperlink ref="AR3" r:id="rId400"/>
-    <hyperlink ref="AR5" r:id="rId401"/>
-    <hyperlink ref="AR6" r:id="rId402"/>
-    <hyperlink ref="AR7" r:id="rId403"/>
-    <hyperlink ref="AR8" r:id="rId404"/>
-    <hyperlink ref="AR9" r:id="rId405"/>
-    <hyperlink ref="AR10" r:id="rId406"/>
-    <hyperlink ref="AR28" r:id="rId407"/>
-    <hyperlink ref="AR27" r:id="rId408"/>
-    <hyperlink ref="AR26" r:id="rId409"/>
-    <hyperlink ref="AR25" r:id="rId410"/>
-    <hyperlink ref="AR24" r:id="rId411"/>
-    <hyperlink ref="AR23" r:id="rId412"/>
-    <hyperlink ref="AR22" r:id="rId413"/>
-    <hyperlink ref="AR21" r:id="rId414"/>
-    <hyperlink ref="AR20" r:id="rId415"/>
-    <hyperlink ref="AR19" r:id="rId416"/>
-    <hyperlink ref="AR18" r:id="rId417"/>
-    <hyperlink ref="AR17" r:id="rId418"/>
-    <hyperlink ref="AR16" r:id="rId419"/>
-    <hyperlink ref="AR15" r:id="rId420"/>
-    <hyperlink ref="AR14" r:id="rId421"/>
-    <hyperlink ref="AR13" r:id="rId422"/>
-    <hyperlink ref="AR12" r:id="rId423"/>
-    <hyperlink ref="AR11" r:id="rId424"/>
-    <hyperlink ref="AD9" r:id="rId425"/>
-    <hyperlink ref="J14" r:id="rId426"/>
-    <hyperlink ref="J8" r:id="rId427"/>
-    <hyperlink ref="J7" r:id="rId428"/>
-    <hyperlink ref="J17" r:id="rId429"/>
-    <hyperlink ref="J18" r:id="rId430"/>
-    <hyperlink ref="J19" r:id="rId431"/>
-    <hyperlink ref="J20" r:id="rId432"/>
-    <hyperlink ref="J21" r:id="rId433"/>
-    <hyperlink ref="J22" r:id="rId434"/>
-    <hyperlink ref="J23" r:id="rId435"/>
-    <hyperlink ref="J24" r:id="rId436"/>
-    <hyperlink ref="J25" r:id="rId437"/>
-    <hyperlink ref="J42" r:id="rId438"/>
-    <hyperlink ref="J43" r:id="rId439"/>
-    <hyperlink ref="J26" r:id="rId440"/>
-    <hyperlink ref="J27" r:id="rId441"/>
-    <hyperlink ref="J62" r:id="rId442"/>
-    <hyperlink ref="J30" r:id="rId443"/>
-    <hyperlink ref="J31" r:id="rId444"/>
-    <hyperlink ref="J32" r:id="rId445"/>
-    <hyperlink ref="J33" r:id="rId446"/>
-    <hyperlink ref="J39" r:id="rId447"/>
-    <hyperlink ref="J70" r:id="rId448"/>
-    <hyperlink ref="J45" r:id="rId449"/>
-    <hyperlink ref="J46" r:id="rId450"/>
-    <hyperlink ref="J47" r:id="rId451"/>
-    <hyperlink ref="J67" r:id="rId452"/>
-    <hyperlink ref="J44" r:id="rId453"/>
-    <hyperlink ref="J48" r:id="rId454"/>
-    <hyperlink ref="J49" r:id="rId455"/>
-    <hyperlink ref="J63" r:id="rId456"/>
-    <hyperlink ref="J64" r:id="rId457"/>
-    <hyperlink ref="J71" r:id="rId458"/>
-    <hyperlink ref="J65" r:id="rId459"/>
-    <hyperlink ref="J34" r:id="rId460"/>
-    <hyperlink ref="J69" r:id="rId461"/>
-    <hyperlink ref="J68" r:id="rId462"/>
-    <hyperlink ref="J66" r:id="rId463"/>
-    <hyperlink ref="J37" r:id="rId464"/>
-    <hyperlink ref="J38" r:id="rId465"/>
-    <hyperlink ref="J29" r:id="rId466"/>
-    <hyperlink ref="J74" r:id="rId467"/>
-    <hyperlink ref="J87" r:id="rId468"/>
-    <hyperlink ref="J41" r:id="rId469"/>
-    <hyperlink ref="J40" r:id="rId470"/>
-    <hyperlink ref="J88" r:id="rId471"/>
-    <hyperlink ref="J89" r:id="rId472"/>
-    <hyperlink ref="J90" r:id="rId473"/>
-    <hyperlink ref="J72" r:id="rId474"/>
-    <hyperlink ref="J91" r:id="rId475"/>
-    <hyperlink ref="J59" r:id="rId476"/>
-    <hyperlink ref="J60" r:id="rId477"/>
-    <hyperlink ref="J35" r:id="rId478"/>
-    <hyperlink ref="J73" r:id="rId479"/>
-    <hyperlink ref="J80" r:id="rId480"/>
-    <hyperlink ref="J75" r:id="rId481"/>
-    <hyperlink ref="J82" r:id="rId482"/>
-    <hyperlink ref="J76" r:id="rId483"/>
-    <hyperlink ref="J83" r:id="rId484"/>
-    <hyperlink ref="J77" r:id="rId485"/>
-    <hyperlink ref="J84" r:id="rId486"/>
-    <hyperlink ref="J78" r:id="rId487"/>
-    <hyperlink ref="J85" r:id="rId488"/>
-    <hyperlink ref="J79" r:id="rId489"/>
-    <hyperlink ref="J81" r:id="rId490"/>
-    <hyperlink ref="J86" r:id="rId491"/>
-    <hyperlink ref="J50" r:id="rId492"/>
-    <hyperlink ref="J103" r:id="rId493"/>
-    <hyperlink ref="J104" r:id="rId494"/>
-    <hyperlink ref="J102" r:id="rId495"/>
-    <hyperlink ref="J99" r:id="rId496"/>
-    <hyperlink ref="J100" r:id="rId497"/>
-    <hyperlink ref="J36" r:id="rId498"/>
-    <hyperlink ref="J101" r:id="rId499"/>
-    <hyperlink ref="J98" r:id="rId500"/>
-    <hyperlink ref="J97" r:id="rId501"/>
-    <hyperlink ref="J96" r:id="rId502"/>
-    <hyperlink ref="J95" r:id="rId503"/>
-    <hyperlink ref="J94" r:id="rId504"/>
-    <hyperlink ref="J93" r:id="rId505"/>
-    <hyperlink ref="J92" r:id="rId506"/>
-    <hyperlink ref="J61" r:id="rId507"/>
-    <hyperlink ref="J58" r:id="rId508"/>
-    <hyperlink ref="J57" r:id="rId509"/>
-    <hyperlink ref="J56" r:id="rId510"/>
-    <hyperlink ref="J55" r:id="rId511"/>
-    <hyperlink ref="J54" r:id="rId512"/>
-    <hyperlink ref="J53" r:id="rId513"/>
-    <hyperlink ref="J52" r:id="rId514"/>
-    <hyperlink ref="J51" r:id="rId515"/>
-    <hyperlink ref="J105" r:id="rId516"/>
-    <hyperlink ref="R27" r:id="rId517"/>
-    <hyperlink ref="R26" r:id="rId518"/>
-    <hyperlink ref="R25" r:id="rId519"/>
-    <hyperlink ref="R24" r:id="rId520"/>
-    <hyperlink ref="R3" r:id="rId521"/>
-    <hyperlink ref="R12" r:id="rId522"/>
-    <hyperlink ref="R13" r:id="rId523"/>
-    <hyperlink ref="R14" r:id="rId524"/>
-    <hyperlink ref="R15" r:id="rId525"/>
-    <hyperlink ref="R16" r:id="rId526"/>
-    <hyperlink ref="R17" r:id="rId527"/>
-    <hyperlink ref="R18" r:id="rId528"/>
-    <hyperlink ref="R19" r:id="rId529"/>
-    <hyperlink ref="R20" r:id="rId530"/>
-    <hyperlink ref="R21" r:id="rId531"/>
-    <hyperlink ref="R5" r:id="rId532"/>
-    <hyperlink ref="R22" r:id="rId533"/>
-    <hyperlink ref="R6" r:id="rId534"/>
-    <hyperlink ref="R7" r:id="rId535"/>
-    <hyperlink ref="R8" r:id="rId536"/>
-    <hyperlink ref="R28" r:id="rId537"/>
-    <hyperlink ref="R10" r:id="rId538"/>
-    <hyperlink ref="R11" r:id="rId539"/>
-    <hyperlink ref="R29" r:id="rId540"/>
-    <hyperlink ref="B30" r:id="rId541"/>
-    <hyperlink ref="T30" r:id="rId542"/>
-    <hyperlink ref="T29" r:id="rId543"/>
-    <hyperlink ref="T28" r:id="rId544" display="http://www.youtube.com/user/motorcyclenewsdotcom"/>
-    <hyperlink ref="T27" r:id="rId545"/>
-    <hyperlink ref="T3" r:id="rId546"/>
-    <hyperlink ref="T16" r:id="rId547"/>
-    <hyperlink ref="T17" r:id="rId548"/>
-    <hyperlink ref="T18" r:id="rId549"/>
-    <hyperlink ref="T19" r:id="rId550"/>
-    <hyperlink ref="T9" r:id="rId551"/>
-    <hyperlink ref="T20" r:id="rId552" display="http://www.youtube.com/user/MINI"/>
-    <hyperlink ref="T21" r:id="rId553" display="http://www.youtube.com/user/thejeepchannel"/>
-    <hyperlink ref="T24" r:id="rId554" display="http://www.youtube.com/user/chevrolet"/>
-    <hyperlink ref="T25" r:id="rId555" display="http://www.youtube.com/user/Ford"/>
-    <hyperlink ref="T26" r:id="rId556" display="http://www.youtube.com/user/BMW"/>
-    <hyperlink ref="T10" r:id="rId557"/>
-    <hyperlink ref="T6" r:id="rId558"/>
-    <hyperlink ref="T11" r:id="rId559"/>
-    <hyperlink ref="T8" r:id="rId560"/>
-    <hyperlink ref="T13" r:id="rId561"/>
-    <hyperlink ref="T31" r:id="rId562"/>
-    <hyperlink ref="T14" r:id="rId563" display="http://www.youtube.com/user/carshowclassic"/>
-    <hyperlink ref="T15" r:id="rId564"/>
-    <hyperlink ref="T32" r:id="rId565"/>
-    <hyperlink ref="T41" r:id="rId566"/>
-    <hyperlink ref="T7" r:id="rId567"/>
-    <hyperlink ref="T5" r:id="rId568"/>
-    <hyperlink ref="T2" r:id="rId569"/>
-    <hyperlink ref="T12" r:id="rId570"/>
-    <hyperlink ref="T34" r:id="rId571"/>
-    <hyperlink ref="T36" r:id="rId572"/>
-    <hyperlink ref="T35" r:id="rId573"/>
-    <hyperlink ref="T37" r:id="rId574"/>
-    <hyperlink ref="T38" r:id="rId575"/>
-    <hyperlink ref="V4" r:id="rId576"/>
-    <hyperlink ref="V9" r:id="rId577"/>
-    <hyperlink ref="V6" r:id="rId578"/>
-    <hyperlink ref="V7" r:id="rId579"/>
-    <hyperlink ref="V8" r:id="rId580"/>
-    <hyperlink ref="V12" r:id="rId581"/>
-    <hyperlink ref="V13" r:id="rId582"/>
-    <hyperlink ref="V14" r:id="rId583"/>
-    <hyperlink ref="V20" r:id="rId584"/>
-    <hyperlink ref="AH6" r:id="rId585"/>
+    <hyperlink ref="AH38" r:id="rId75"/>
+    <hyperlink ref="X6" r:id="rId76"/>
+    <hyperlink ref="AH37" r:id="rId77"/>
+    <hyperlink ref="D17" r:id="rId78"/>
+    <hyperlink ref="D18" r:id="rId79"/>
+    <hyperlink ref="D19" r:id="rId80"/>
+    <hyperlink ref="D20" r:id="rId81"/>
+    <hyperlink ref="D21" r:id="rId82"/>
+    <hyperlink ref="D22" r:id="rId83"/>
+    <hyperlink ref="N2" r:id="rId84"/>
+    <hyperlink ref="N3" r:id="rId85"/>
+    <hyperlink ref="N4" r:id="rId86"/>
+    <hyperlink ref="N6" r:id="rId87"/>
+    <hyperlink ref="N10" r:id="rId88"/>
+    <hyperlink ref="N11" r:id="rId89"/>
+    <hyperlink ref="N12" r:id="rId90"/>
+    <hyperlink ref="N13" r:id="rId91"/>
+    <hyperlink ref="N14" r:id="rId92"/>
+    <hyperlink ref="N28" r:id="rId93"/>
+    <hyperlink ref="N20" r:id="rId94"/>
+    <hyperlink ref="N21" r:id="rId95"/>
+    <hyperlink ref="N22" r:id="rId96"/>
+    <hyperlink ref="N24" r:id="rId97"/>
+    <hyperlink ref="N25" r:id="rId98"/>
+    <hyperlink ref="N26" r:id="rId99"/>
+    <hyperlink ref="N27" r:id="rId100"/>
+    <hyperlink ref="N34" r:id="rId101"/>
+    <hyperlink ref="N39" r:id="rId102"/>
+    <hyperlink ref="N36" r:id="rId103"/>
+    <hyperlink ref="N37" r:id="rId104"/>
+    <hyperlink ref="N38" r:id="rId105"/>
+    <hyperlink ref="N16" r:id="rId106"/>
+    <hyperlink ref="N17" r:id="rId107"/>
+    <hyperlink ref="N18" r:id="rId108"/>
+    <hyperlink ref="N23" r:id="rId109"/>
+    <hyperlink ref="N19" r:id="rId110"/>
+    <hyperlink ref="N7" r:id="rId111"/>
+    <hyperlink ref="N8" r:id="rId112"/>
+    <hyperlink ref="N15" r:id="rId113"/>
+    <hyperlink ref="N44" r:id="rId114"/>
+    <hyperlink ref="N29" r:id="rId115"/>
+    <hyperlink ref="N30" r:id="rId116"/>
+    <hyperlink ref="N32" r:id="rId117"/>
+    <hyperlink ref="N33" r:id="rId118"/>
+    <hyperlink ref="N35" r:id="rId119"/>
+    <hyperlink ref="N40" r:id="rId120"/>
+    <hyperlink ref="N41" r:id="rId121"/>
+    <hyperlink ref="N45" r:id="rId122"/>
+    <hyperlink ref="N46" r:id="rId123"/>
+    <hyperlink ref="N42" r:id="rId124"/>
+    <hyperlink ref="N43" r:id="rId125"/>
+    <hyperlink ref="N47" r:id="rId126"/>
+    <hyperlink ref="N48" r:id="rId127"/>
+    <hyperlink ref="N49" r:id="rId128"/>
+    <hyperlink ref="N50" r:id="rId129"/>
+    <hyperlink ref="N51" r:id="rId130"/>
+    <hyperlink ref="N53" r:id="rId131"/>
+    <hyperlink ref="N54" r:id="rId132"/>
+    <hyperlink ref="N55" r:id="rId133"/>
+    <hyperlink ref="N56" r:id="rId134"/>
+    <hyperlink ref="N57" r:id="rId135"/>
+    <hyperlink ref="N58" r:id="rId136"/>
+    <hyperlink ref="N59" r:id="rId137"/>
+    <hyperlink ref="N60" r:id="rId138"/>
+    <hyperlink ref="N62" r:id="rId139"/>
+    <hyperlink ref="N63" r:id="rId140"/>
+    <hyperlink ref="N64" r:id="rId141"/>
+    <hyperlink ref="N65" r:id="rId142"/>
+    <hyperlink ref="N66" r:id="rId143"/>
+    <hyperlink ref="N69" r:id="rId144"/>
+    <hyperlink ref="N67" r:id="rId145"/>
+    <hyperlink ref="N68" r:id="rId146"/>
+    <hyperlink ref="N70" r:id="rId147"/>
+    <hyperlink ref="B19" r:id="rId148"/>
+    <hyperlink ref="B20" r:id="rId149"/>
+    <hyperlink ref="B21" r:id="rId150"/>
+    <hyperlink ref="V15" r:id="rId151"/>
+    <hyperlink ref="V10" r:id="rId152"/>
+    <hyperlink ref="V11" r:id="rId153"/>
+    <hyperlink ref="V16" r:id="rId154"/>
+    <hyperlink ref="V18" r:id="rId155"/>
+    <hyperlink ref="V17" r:id="rId156"/>
+    <hyperlink ref="V19" r:id="rId157"/>
+    <hyperlink ref="H3" r:id="rId158"/>
+    <hyperlink ref="H8" r:id="rId159"/>
+    <hyperlink ref="H11" r:id="rId160"/>
+    <hyperlink ref="H47" r:id="rId161"/>
+    <hyperlink ref="H12" r:id="rId162"/>
+    <hyperlink ref="H31" r:id="rId163"/>
+    <hyperlink ref="H34" r:id="rId164"/>
+    <hyperlink ref="H36" r:id="rId165"/>
+    <hyperlink ref="H37" r:id="rId166"/>
+    <hyperlink ref="H39" r:id="rId167"/>
+    <hyperlink ref="H6" r:id="rId168"/>
+    <hyperlink ref="H38" r:id="rId169"/>
+    <hyperlink ref="H43" r:id="rId170"/>
+    <hyperlink ref="H42" r:id="rId171"/>
+    <hyperlink ref="H41" r:id="rId172"/>
+    <hyperlink ref="H54" r:id="rId173"/>
+    <hyperlink ref="H2" r:id="rId174"/>
+    <hyperlink ref="H7" r:id="rId175"/>
+    <hyperlink ref="H4" r:id="rId176"/>
+    <hyperlink ref="AF27" r:id="rId177"/>
+    <hyperlink ref="AF34" r:id="rId178"/>
+    <hyperlink ref="AF35" r:id="rId179"/>
+    <hyperlink ref="AF5" r:id="rId180"/>
+    <hyperlink ref="AF32" r:id="rId181"/>
+    <hyperlink ref="AF33" r:id="rId182"/>
+    <hyperlink ref="AF28" r:id="rId183"/>
+    <hyperlink ref="AF6" r:id="rId184"/>
+    <hyperlink ref="AF3" r:id="rId185"/>
+    <hyperlink ref="AF4" r:id="rId186"/>
+    <hyperlink ref="AF2" r:id="rId187"/>
+    <hyperlink ref="AF30" r:id="rId188"/>
+    <hyperlink ref="AF8" r:id="rId189"/>
+    <hyperlink ref="AF7" r:id="rId190"/>
+    <hyperlink ref="AF29" r:id="rId191"/>
+    <hyperlink ref="AF20" r:id="rId192"/>
+    <hyperlink ref="AF9" r:id="rId193"/>
+    <hyperlink ref="AF11" r:id="rId194"/>
+    <hyperlink ref="AF12" r:id="rId195"/>
+    <hyperlink ref="AF13" r:id="rId196"/>
+    <hyperlink ref="AF14" r:id="rId197"/>
+    <hyperlink ref="AF15" r:id="rId198"/>
+    <hyperlink ref="AF16" r:id="rId199"/>
+    <hyperlink ref="AF17" r:id="rId200"/>
+    <hyperlink ref="AF21" r:id="rId201"/>
+    <hyperlink ref="AF23" r:id="rId202"/>
+    <hyperlink ref="AF18" r:id="rId203"/>
+    <hyperlink ref="AF24" r:id="rId204"/>
+    <hyperlink ref="AF19" r:id="rId205"/>
+    <hyperlink ref="AF22" r:id="rId206"/>
+    <hyperlink ref="AF25" r:id="rId207"/>
+    <hyperlink ref="AF26" r:id="rId208"/>
+    <hyperlink ref="AF10" r:id="rId209"/>
+    <hyperlink ref="AF31" r:id="rId210"/>
+    <hyperlink ref="H68" r:id="rId211"/>
+    <hyperlink ref="H62" r:id="rId212"/>
+    <hyperlink ref="H61" r:id="rId213"/>
+    <hyperlink ref="H73" r:id="rId214"/>
+    <hyperlink ref="H59" r:id="rId215"/>
+    <hyperlink ref="H60" r:id="rId216"/>
+    <hyperlink ref="H65" r:id="rId217"/>
+    <hyperlink ref="H67" r:id="rId218"/>
+    <hyperlink ref="H66" r:id="rId219"/>
+    <hyperlink ref="H69" r:id="rId220"/>
+    <hyperlink ref="H64" r:id="rId221"/>
+    <hyperlink ref="H70" r:id="rId222"/>
+    <hyperlink ref="H72" r:id="rId223"/>
+    <hyperlink ref="H63" r:id="rId224"/>
+    <hyperlink ref="H71" r:id="rId225"/>
+    <hyperlink ref="H51" r:id="rId226"/>
+    <hyperlink ref="H46" r:id="rId227"/>
+    <hyperlink ref="H40" r:id="rId228"/>
+    <hyperlink ref="H76" r:id="rId229"/>
+    <hyperlink ref="H32" r:id="rId230"/>
+    <hyperlink ref="H15" r:id="rId231"/>
+    <hyperlink ref="H16" r:id="rId232"/>
+    <hyperlink ref="H17" r:id="rId233"/>
+    <hyperlink ref="H5" r:id="rId234"/>
+    <hyperlink ref="H10" r:id="rId235"/>
+    <hyperlink ref="H56" r:id="rId236"/>
+    <hyperlink ref="H35" r:id="rId237"/>
+    <hyperlink ref="H77" r:id="rId238"/>
+    <hyperlink ref="H78" r:id="rId239"/>
+    <hyperlink ref="H57" r:id="rId240"/>
+    <hyperlink ref="F12" r:id="rId241"/>
+    <hyperlink ref="B25" r:id="rId242"/>
+    <hyperlink ref="AD10" r:id="rId243"/>
+    <hyperlink ref="F13" r:id="rId244"/>
+    <hyperlink ref="AD11" r:id="rId245"/>
+    <hyperlink ref="AD12" r:id="rId246"/>
+    <hyperlink ref="F14" r:id="rId247"/>
+    <hyperlink ref="H58" r:id="rId248"/>
+    <hyperlink ref="V2" r:id="rId249"/>
+    <hyperlink ref="V3" r:id="rId250"/>
+    <hyperlink ref="AL27" r:id="rId251"/>
+    <hyperlink ref="AL28" r:id="rId252"/>
+    <hyperlink ref="AL29" r:id="rId253"/>
+    <hyperlink ref="X9" r:id="rId254"/>
+    <hyperlink ref="X8" r:id="rId255"/>
+    <hyperlink ref="X7" r:id="rId256"/>
+    <hyperlink ref="H44" r:id="rId257"/>
+    <hyperlink ref="R9" r:id="rId258" display="http://www.youtube.com/user/motorstelevision"/>
+    <hyperlink ref="B26" r:id="rId259"/>
+    <hyperlink ref="B27" r:id="rId260"/>
+    <hyperlink ref="H52" r:id="rId261"/>
+    <hyperlink ref="H49" r:id="rId262"/>
+    <hyperlink ref="H50" r:id="rId263"/>
+    <hyperlink ref="AH18" r:id="rId264"/>
+    <hyperlink ref="AH19" r:id="rId265"/>
+    <hyperlink ref="AH20" r:id="rId266"/>
+    <hyperlink ref="AH28" r:id="rId267"/>
+    <hyperlink ref="AH29" r:id="rId268"/>
+    <hyperlink ref="AH30" r:id="rId269"/>
+    <hyperlink ref="AH31" r:id="rId270"/>
+    <hyperlink ref="AH32" r:id="rId271"/>
+    <hyperlink ref="AH33" r:id="rId272"/>
+    <hyperlink ref="AH10" r:id="rId273"/>
+    <hyperlink ref="AH11" r:id="rId274"/>
+    <hyperlink ref="AH54" r:id="rId275"/>
+    <hyperlink ref="AH66" r:id="rId276"/>
+    <hyperlink ref="AH55" r:id="rId277"/>
+    <hyperlink ref="AH56" r:id="rId278"/>
+    <hyperlink ref="AH67" r:id="rId279"/>
+    <hyperlink ref="AH59" r:id="rId280"/>
+    <hyperlink ref="AH64" r:id="rId281"/>
+    <hyperlink ref="AH34" r:id="rId282"/>
+    <hyperlink ref="AH35" r:id="rId283"/>
+    <hyperlink ref="X2" r:id="rId284"/>
+    <hyperlink ref="X3" r:id="rId285"/>
+    <hyperlink ref="AD15" r:id="rId286"/>
+    <hyperlink ref="AD16" r:id="rId287"/>
+    <hyperlink ref="AD17" r:id="rId288"/>
+    <hyperlink ref="AD18" r:id="rId289"/>
+    <hyperlink ref="AD19" r:id="rId290"/>
+    <hyperlink ref="AD20" r:id="rId291"/>
+    <hyperlink ref="AD21" r:id="rId292"/>
+    <hyperlink ref="AD23" r:id="rId293"/>
+    <hyperlink ref="AD13" r:id="rId294"/>
+    <hyperlink ref="AD24" r:id="rId295"/>
+    <hyperlink ref="AD14" r:id="rId296"/>
+    <hyperlink ref="AD25" r:id="rId297"/>
+    <hyperlink ref="AD27" r:id="rId298"/>
+    <hyperlink ref="AD26" r:id="rId299"/>
+    <hyperlink ref="AH12" r:id="rId300"/>
+    <hyperlink ref="AH60" r:id="rId301"/>
+    <hyperlink ref="AH63" r:id="rId302"/>
+    <hyperlink ref="AH57" r:id="rId303"/>
+    <hyperlink ref="AH58" r:id="rId304"/>
+    <hyperlink ref="AH62" r:id="rId305"/>
+    <hyperlink ref="AH61" r:id="rId306"/>
+    <hyperlink ref="AH65" r:id="rId307"/>
+    <hyperlink ref="AN12" r:id="rId308"/>
+    <hyperlink ref="AN14" r:id="rId309"/>
+    <hyperlink ref="AN24" r:id="rId310"/>
+    <hyperlink ref="AN19" r:id="rId311"/>
+    <hyperlink ref="AN13" r:id="rId312"/>
+    <hyperlink ref="AN15" r:id="rId313"/>
+    <hyperlink ref="AN17" r:id="rId314"/>
+    <hyperlink ref="AN16" r:id="rId315"/>
+    <hyperlink ref="AN18" r:id="rId316"/>
+    <hyperlink ref="AN20" r:id="rId317"/>
+    <hyperlink ref="AN21" r:id="rId318"/>
+    <hyperlink ref="AN22" r:id="rId319"/>
+    <hyperlink ref="AN23" r:id="rId320"/>
+    <hyperlink ref="AN25" r:id="rId321"/>
+    <hyperlink ref="AD28" r:id="rId322"/>
+    <hyperlink ref="AD29" r:id="rId323"/>
+    <hyperlink ref="H9" r:id="rId324"/>
+    <hyperlink ref="H29" r:id="rId325"/>
+    <hyperlink ref="H30" r:id="rId326"/>
+    <hyperlink ref="H19" r:id="rId327"/>
+    <hyperlink ref="H14" r:id="rId328"/>
+    <hyperlink ref="H21" r:id="rId329"/>
+    <hyperlink ref="H20" r:id="rId330"/>
+    <hyperlink ref="H13" r:id="rId331"/>
+    <hyperlink ref="H22" r:id="rId332"/>
+    <hyperlink ref="H23" r:id="rId333"/>
+    <hyperlink ref="H24" r:id="rId334"/>
+    <hyperlink ref="AL10" r:id="rId335"/>
+    <hyperlink ref="AL11" r:id="rId336"/>
+    <hyperlink ref="AL19" r:id="rId337"/>
+    <hyperlink ref="AL12" r:id="rId338"/>
+    <hyperlink ref="AL21" r:id="rId339"/>
+    <hyperlink ref="AL13" r:id="rId340"/>
+    <hyperlink ref="AL22" r:id="rId341"/>
+    <hyperlink ref="AL14" r:id="rId342"/>
+    <hyperlink ref="AL23" r:id="rId343"/>
+    <hyperlink ref="AL15" r:id="rId344"/>
+    <hyperlink ref="AL16" r:id="rId345"/>
+    <hyperlink ref="AL17" r:id="rId346"/>
+    <hyperlink ref="AL18" r:id="rId347"/>
+    <hyperlink ref="AL24" r:id="rId348"/>
+    <hyperlink ref="AL25" r:id="rId349"/>
+    <hyperlink ref="AL20" r:id="rId350"/>
+    <hyperlink ref="AL9" r:id="rId351"/>
+    <hyperlink ref="R23" r:id="rId352" display="http://www.youtube.com/user/MINI"/>
+    <hyperlink ref="R30" r:id="rId353" display="http://www.youtube.com/user/motousa"/>
+    <hyperlink ref="R32" r:id="rId354" display="http://www.youtube.com/user/autocar"/>
+    <hyperlink ref="R33" r:id="rId355" display="http://www.youtube.com/user/TopGear"/>
+    <hyperlink ref="R34" r:id="rId356" display="http://www.youtube.com/user/motorstelevision"/>
+    <hyperlink ref="R37" r:id="rId357" display="http://www.youtube.com/user/militarychannel"/>
+    <hyperlink ref="R38" r:id="rId358" display="http://www.youtube.com/user/carshowclassic"/>
+    <hyperlink ref="R39" r:id="rId359" display="http://www.youtube.com/user/Motorscouk"/>
+    <hyperlink ref="R40" r:id="rId360" display="http://www.youtube.com/user/EmiratesExperience"/>
+    <hyperlink ref="R42" r:id="rId361" display="http://www.youtube.com/user/rockitoutblog"/>
+    <hyperlink ref="R43" r:id="rId362" display="http://www.youtube.com/user/musiciansinstitute"/>
+    <hyperlink ref="R44" r:id="rId363" display="http://www.youtube.com/user/GuitarCenterTV"/>
+    <hyperlink ref="R46" r:id="rId364" display="http://www.youtube.com/user/TylerWardMusic"/>
+    <hyperlink ref="AJ17" r:id="rId365"/>
+    <hyperlink ref="AJ23" r:id="rId366"/>
+    <hyperlink ref="AJ24" r:id="rId367"/>
+    <hyperlink ref="AJ25" r:id="rId368"/>
+    <hyperlink ref="AJ26" r:id="rId369"/>
+    <hyperlink ref="AJ27" r:id="rId370"/>
+    <hyperlink ref="AJ22" r:id="rId371"/>
+    <hyperlink ref="AJ30" r:id="rId372"/>
+    <hyperlink ref="AJ29" r:id="rId373"/>
+    <hyperlink ref="AJ28" r:id="rId374"/>
+    <hyperlink ref="AJ18" r:id="rId375"/>
+    <hyperlink ref="AJ21" r:id="rId376"/>
+    <hyperlink ref="AJ35" r:id="rId377"/>
+    <hyperlink ref="AJ36" r:id="rId378"/>
+    <hyperlink ref="AD30" r:id="rId379"/>
+    <hyperlink ref="AJ32" r:id="rId380"/>
+    <hyperlink ref="AJ33" r:id="rId381"/>
+    <hyperlink ref="AJ31" r:id="rId382"/>
+    <hyperlink ref="AJ34" r:id="rId383"/>
+    <hyperlink ref="AJ37" r:id="rId384"/>
+    <hyperlink ref="AP2" r:id="rId385"/>
+    <hyperlink ref="AP4" r:id="rId386"/>
+    <hyperlink ref="AP5" r:id="rId387"/>
+    <hyperlink ref="AP6" r:id="rId388"/>
+    <hyperlink ref="AP9" r:id="rId389"/>
+    <hyperlink ref="AP10" r:id="rId390"/>
+    <hyperlink ref="AP12" r:id="rId391"/>
+    <hyperlink ref="AP11" r:id="rId392"/>
+    <hyperlink ref="AP13" r:id="rId393"/>
+    <hyperlink ref="AP15" r:id="rId394"/>
+    <hyperlink ref="AP14" r:id="rId395"/>
+    <hyperlink ref="B24" r:id="rId396"/>
+    <hyperlink ref="B22" r:id="rId397"/>
+    <hyperlink ref="AR2" r:id="rId398"/>
+    <hyperlink ref="AR3" r:id="rId399"/>
+    <hyperlink ref="AR5" r:id="rId400"/>
+    <hyperlink ref="AR6" r:id="rId401"/>
+    <hyperlink ref="AR7" r:id="rId402"/>
+    <hyperlink ref="AR8" r:id="rId403"/>
+    <hyperlink ref="AR9" r:id="rId404"/>
+    <hyperlink ref="AR10" r:id="rId405"/>
+    <hyperlink ref="AR28" r:id="rId406"/>
+    <hyperlink ref="AR27" r:id="rId407"/>
+    <hyperlink ref="AR26" r:id="rId408"/>
+    <hyperlink ref="AR25" r:id="rId409"/>
+    <hyperlink ref="AR24" r:id="rId410"/>
+    <hyperlink ref="AR23" r:id="rId411"/>
+    <hyperlink ref="AR22" r:id="rId412"/>
+    <hyperlink ref="AR21" r:id="rId413"/>
+    <hyperlink ref="AR20" r:id="rId414"/>
+    <hyperlink ref="AR19" r:id="rId415"/>
+    <hyperlink ref="AR18" r:id="rId416"/>
+    <hyperlink ref="AR17" r:id="rId417"/>
+    <hyperlink ref="AR16" r:id="rId418"/>
+    <hyperlink ref="AR15" r:id="rId419"/>
+    <hyperlink ref="AR14" r:id="rId420"/>
+    <hyperlink ref="AR13" r:id="rId421"/>
+    <hyperlink ref="AR12" r:id="rId422"/>
+    <hyperlink ref="AR11" r:id="rId423"/>
+    <hyperlink ref="AD9" r:id="rId424"/>
+    <hyperlink ref="J14" r:id="rId425"/>
+    <hyperlink ref="J8" r:id="rId426"/>
+    <hyperlink ref="J7" r:id="rId427"/>
+    <hyperlink ref="J17" r:id="rId428"/>
+    <hyperlink ref="J18" r:id="rId429"/>
+    <hyperlink ref="J19" r:id="rId430"/>
+    <hyperlink ref="J20" r:id="rId431"/>
+    <hyperlink ref="J21" r:id="rId432"/>
+    <hyperlink ref="J22" r:id="rId433"/>
+    <hyperlink ref="J23" r:id="rId434"/>
+    <hyperlink ref="J24" r:id="rId435"/>
+    <hyperlink ref="J25" r:id="rId436"/>
+    <hyperlink ref="J42" r:id="rId437"/>
+    <hyperlink ref="J43" r:id="rId438"/>
+    <hyperlink ref="J26" r:id="rId439"/>
+    <hyperlink ref="J27" r:id="rId440"/>
+    <hyperlink ref="J62" r:id="rId441"/>
+    <hyperlink ref="J30" r:id="rId442"/>
+    <hyperlink ref="J31" r:id="rId443"/>
+    <hyperlink ref="J32" r:id="rId444"/>
+    <hyperlink ref="J33" r:id="rId445"/>
+    <hyperlink ref="J39" r:id="rId446"/>
+    <hyperlink ref="J70" r:id="rId447"/>
+    <hyperlink ref="J45" r:id="rId448"/>
+    <hyperlink ref="J46" r:id="rId449"/>
+    <hyperlink ref="J47" r:id="rId450"/>
+    <hyperlink ref="J67" r:id="rId451"/>
+    <hyperlink ref="J44" r:id="rId452"/>
+    <hyperlink ref="J48" r:id="rId453"/>
+    <hyperlink ref="J49" r:id="rId454"/>
+    <hyperlink ref="J63" r:id="rId455"/>
+    <hyperlink ref="J64" r:id="rId456"/>
+    <hyperlink ref="J71" r:id="rId457"/>
+    <hyperlink ref="J65" r:id="rId458"/>
+    <hyperlink ref="J34" r:id="rId459"/>
+    <hyperlink ref="J69" r:id="rId460"/>
+    <hyperlink ref="J68" r:id="rId461"/>
+    <hyperlink ref="J66" r:id="rId462"/>
+    <hyperlink ref="J37" r:id="rId463"/>
+    <hyperlink ref="J38" r:id="rId464"/>
+    <hyperlink ref="J29" r:id="rId465"/>
+    <hyperlink ref="J74" r:id="rId466"/>
+    <hyperlink ref="J87" r:id="rId467"/>
+    <hyperlink ref="J41" r:id="rId468"/>
+    <hyperlink ref="J40" r:id="rId469"/>
+    <hyperlink ref="J88" r:id="rId470"/>
+    <hyperlink ref="J89" r:id="rId471"/>
+    <hyperlink ref="J90" r:id="rId472"/>
+    <hyperlink ref="J72" r:id="rId473"/>
+    <hyperlink ref="J91" r:id="rId474"/>
+    <hyperlink ref="J59" r:id="rId475"/>
+    <hyperlink ref="J60" r:id="rId476"/>
+    <hyperlink ref="J35" r:id="rId477"/>
+    <hyperlink ref="J73" r:id="rId478"/>
+    <hyperlink ref="J80" r:id="rId479"/>
+    <hyperlink ref="J75" r:id="rId480"/>
+    <hyperlink ref="J82" r:id="rId481"/>
+    <hyperlink ref="J76" r:id="rId482"/>
+    <hyperlink ref="J83" r:id="rId483"/>
+    <hyperlink ref="J77" r:id="rId484"/>
+    <hyperlink ref="J84" r:id="rId485"/>
+    <hyperlink ref="J78" r:id="rId486"/>
+    <hyperlink ref="J85" r:id="rId487"/>
+    <hyperlink ref="J79" r:id="rId488"/>
+    <hyperlink ref="J81" r:id="rId489"/>
+    <hyperlink ref="J86" r:id="rId490"/>
+    <hyperlink ref="J50" r:id="rId491"/>
+    <hyperlink ref="J103" r:id="rId492"/>
+    <hyperlink ref="J104" r:id="rId493"/>
+    <hyperlink ref="J102" r:id="rId494"/>
+    <hyperlink ref="J99" r:id="rId495"/>
+    <hyperlink ref="J100" r:id="rId496"/>
+    <hyperlink ref="J36" r:id="rId497"/>
+    <hyperlink ref="J101" r:id="rId498"/>
+    <hyperlink ref="J98" r:id="rId499"/>
+    <hyperlink ref="J97" r:id="rId500"/>
+    <hyperlink ref="J96" r:id="rId501"/>
+    <hyperlink ref="J95" r:id="rId502"/>
+    <hyperlink ref="J94" r:id="rId503"/>
+    <hyperlink ref="J93" r:id="rId504"/>
+    <hyperlink ref="J92" r:id="rId505"/>
+    <hyperlink ref="J61" r:id="rId506"/>
+    <hyperlink ref="J58" r:id="rId507"/>
+    <hyperlink ref="J57" r:id="rId508"/>
+    <hyperlink ref="J56" r:id="rId509"/>
+    <hyperlink ref="J55" r:id="rId510"/>
+    <hyperlink ref="J54" r:id="rId511"/>
+    <hyperlink ref="J53" r:id="rId512"/>
+    <hyperlink ref="J52" r:id="rId513"/>
+    <hyperlink ref="J51" r:id="rId514"/>
+    <hyperlink ref="J105" r:id="rId515"/>
+    <hyperlink ref="R27" r:id="rId516"/>
+    <hyperlink ref="R26" r:id="rId517"/>
+    <hyperlink ref="R25" r:id="rId518"/>
+    <hyperlink ref="R24" r:id="rId519"/>
+    <hyperlink ref="R3" r:id="rId520"/>
+    <hyperlink ref="R12" r:id="rId521"/>
+    <hyperlink ref="R13" r:id="rId522"/>
+    <hyperlink ref="R14" r:id="rId523"/>
+    <hyperlink ref="R15" r:id="rId524"/>
+    <hyperlink ref="R16" r:id="rId525"/>
+    <hyperlink ref="R17" r:id="rId526"/>
+    <hyperlink ref="R18" r:id="rId527"/>
+    <hyperlink ref="R19" r:id="rId528"/>
+    <hyperlink ref="R20" r:id="rId529"/>
+    <hyperlink ref="R21" r:id="rId530"/>
+    <hyperlink ref="R5" r:id="rId531"/>
+    <hyperlink ref="R22" r:id="rId532"/>
+    <hyperlink ref="R6" r:id="rId533"/>
+    <hyperlink ref="R7" r:id="rId534"/>
+    <hyperlink ref="R8" r:id="rId535"/>
+    <hyperlink ref="R28" r:id="rId536"/>
+    <hyperlink ref="R10" r:id="rId537"/>
+    <hyperlink ref="R11" r:id="rId538"/>
+    <hyperlink ref="R29" r:id="rId539"/>
+    <hyperlink ref="B30" r:id="rId540"/>
+    <hyperlink ref="T30" r:id="rId541"/>
+    <hyperlink ref="T29" r:id="rId542"/>
+    <hyperlink ref="T28" r:id="rId543" display="http://www.youtube.com/user/motorcyclenewsdotcom"/>
+    <hyperlink ref="T27" r:id="rId544"/>
+    <hyperlink ref="T3" r:id="rId545"/>
+    <hyperlink ref="T16" r:id="rId546"/>
+    <hyperlink ref="T17" r:id="rId547"/>
+    <hyperlink ref="T18" r:id="rId548"/>
+    <hyperlink ref="T19" r:id="rId549"/>
+    <hyperlink ref="T9" r:id="rId550"/>
+    <hyperlink ref="T20" r:id="rId551" display="http://www.youtube.com/user/MINI"/>
+    <hyperlink ref="T21" r:id="rId552" display="http://www.youtube.com/user/thejeepchannel"/>
+    <hyperlink ref="T24" r:id="rId553" display="http://www.youtube.com/user/chevrolet"/>
+    <hyperlink ref="T25" r:id="rId554" display="http://www.youtube.com/user/Ford"/>
+    <hyperlink ref="T26" r:id="rId555" display="http://www.youtube.com/user/BMW"/>
+    <hyperlink ref="T10" r:id="rId556"/>
+    <hyperlink ref="T6" r:id="rId557"/>
+    <hyperlink ref="T11" r:id="rId558"/>
+    <hyperlink ref="T8" r:id="rId559"/>
+    <hyperlink ref="T13" r:id="rId560"/>
+    <hyperlink ref="T31" r:id="rId561"/>
+    <hyperlink ref="T14" r:id="rId562" display="http://www.youtube.com/user/carshowclassic"/>
+    <hyperlink ref="T15" r:id="rId563"/>
+    <hyperlink ref="T32" r:id="rId564"/>
+    <hyperlink ref="T41" r:id="rId565"/>
+    <hyperlink ref="T7" r:id="rId566"/>
+    <hyperlink ref="T5" r:id="rId567"/>
+    <hyperlink ref="T2" r:id="rId568"/>
+    <hyperlink ref="T12" r:id="rId569"/>
+    <hyperlink ref="T34" r:id="rId570"/>
+    <hyperlink ref="T36" r:id="rId571"/>
+    <hyperlink ref="T35" r:id="rId572"/>
+    <hyperlink ref="T37" r:id="rId573"/>
+    <hyperlink ref="T38" r:id="rId574"/>
+    <hyperlink ref="V4" r:id="rId575"/>
+    <hyperlink ref="V9" r:id="rId576"/>
+    <hyperlink ref="V6" r:id="rId577"/>
+    <hyperlink ref="V7" r:id="rId578"/>
+    <hyperlink ref="V8" r:id="rId579"/>
+    <hyperlink ref="V12" r:id="rId580"/>
+    <hyperlink ref="V13" r:id="rId581"/>
+    <hyperlink ref="V14" r:id="rId582"/>
+    <hyperlink ref="V20" r:id="rId583"/>
+    <hyperlink ref="AH6" r:id="rId584"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -12542,7 +12542,7 @@
     </row>
     <row r="8" spans="1:1" ht="16.2">
       <c r="A8" s="77" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="16.2">

</xml_diff>

<commit_message>
youtube lib, check invalid stuff from utube; don't save any recently watched channel if channel id is zero; channelLineup recentlywatched is empty
git-svn-id: https://everest.teltel.com:8443/repos/misc/web/nnvmso@2143 a0a5f996-2bb4-401c-8778-395c3c01700f
</commit_message>
<xml_diff>
--- a/war/WEB-INF/views/admin/CSets.xlsx
+++ b/war/WEB-INF/views/admin/CSets.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1583" uniqueCount="1360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1584" uniqueCount="1361">
   <si>
     <t>Top Level Categories</t>
   </si>
@@ -4769,6 +4769,9 @@
   </si>
   <si>
     <t>http://www.maplestage.net/show/流行in House /</t>
+  </si>
+  <si>
+    <t>http://www.maplestage.net/drama/愛讓我們在一起/</t>
   </si>
 </sst>
 </file>
@@ -5163,7 +5166,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5348,6 +5351,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="118" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="120">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
@@ -6617,8 +6621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AR106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
-      <selection activeCell="AJ13" sqref="AJ13"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.95" customHeight="1"/>
@@ -9172,9 +9176,8 @@
       <c r="K22" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="L22" s="37" t="str">
-        <f>HYPERLINK("http://www.maplestage.net/drama/%E6%84%9B%E8%AE%93%E6%88%91%E5%80%91%E5%9C%A8%E4%B8%80%E8%B5%B7","http://www.maplestage.net/drama/愛讓我們在一起")</f>
-        <v>http://www.maplestage.net/drama/愛讓我們在一起</v>
+      <c r="L22" s="78" t="s">
+        <v>1360</v>
       </c>
       <c r="M22" s="36" t="s">
         <v>236</v>
@@ -12343,6 +12346,7 @@
     <hyperlink ref="V14" r:id="rId582"/>
     <hyperlink ref="V20" r:id="rId583"/>
     <hyperlink ref="AH6" r:id="rId584"/>
+    <hyperlink ref="L22" r:id="rId585"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>